<commit_message>
Zeitblätter auf Stand gebracht, Projektplan Zeiten eingetragen
</commit_message>
<xml_diff>
--- a/Projekt Handbuch/Projektplan.xlsx
+++ b/Projekt Handbuch/Projektplan.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ursus/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Documents\Eigene Daten\#Master_3\S1 Kopplung\GitHub AlienHacky\Projekt Handbuch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
     <author>Stefan Hagen</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP13" authorId="0">
+    <comment ref="AP13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -361,7 +361,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0_ ;[Red]\-0.0\ "/>
   </numFmts>
@@ -681,6 +681,9 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -702,12 +705,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1175,109 +1175,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AP64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" customWidth="1"/>
     <col min="3" max="6" width="4" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="4" style="1" customWidth="1"/>
-    <col min="13" max="17" width="5.5" style="1" customWidth="1"/>
-    <col min="18" max="40" width="3.6640625" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="11.5" style="1"/>
+    <col min="13" max="17" width="5.42578125" style="1" customWidth="1"/>
+    <col min="18" max="40" width="3.7109375" style="1" customWidth="1"/>
+    <col min="41" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:42" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:42" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="47" t="s">
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="46">
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="47">
         <v>2016</v>
       </c>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="46"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="46"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="46">
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="47"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="47"/>
+      <c r="AE8" s="47"/>
+      <c r="AF8" s="47">
         <v>2017</v>
       </c>
-      <c r="AG8" s="46"/>
-      <c r="AH8" s="46"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="46"/>
-      <c r="AK8" s="46"/>
-      <c r="AL8" s="46"/>
-      <c r="AM8" s="46"/>
-      <c r="AN8" s="46"/>
-    </row>
-    <row r="9" spans="1:42" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="44"/>
-      <c r="B9" s="43"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="47"/>
+      <c r="AJ8" s="47"/>
+      <c r="AK8" s="47"/>
+      <c r="AL8" s="47"/>
+      <c r="AM8" s="47"/>
+      <c r="AN8" s="47"/>
+    </row>
+    <row r="9" spans="1:42" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="45"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>5</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="AM10" s="22"/>
       <c r="AN10" s="22"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>7</v>
       </c>
@@ -1541,7 +1541,7 @@
       <c r="AM11" s="22"/>
       <c r="AN11" s="22"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>6</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="AM12" s="22"/>
       <c r="AN12" s="22"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>8</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
@@ -1773,7 +1773,7 @@
       <c r="AM14" s="22"/>
       <c r="AN14" s="22"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="AM15" s="22"/>
       <c r="AN15" s="22"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>70</v>
       </c>
@@ -1925,7 +1925,7 @@
       <c r="AM16" s="22"/>
       <c r="AN16" s="22"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="25"/>
       <c r="C17" s="17"/>
@@ -1967,7 +1967,7 @@
       <c r="AM17" s="22"/>
       <c r="AN17" s="22"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>11</v>
       </c>
@@ -2016,7 +2016,7 @@
       <c r="AM18" s="22"/>
       <c r="AN18" s="22"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
@@ -2036,10 +2036,12 @@
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="K19" s="17">
+        <v>1</v>
+      </c>
       <c r="L19" s="9">
         <f t="shared" ref="L19:L26" si="6">SUM(H19:K19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" ref="M19:P26" si="7">H19-C19</f>
@@ -2055,11 +2057,11 @@
       </c>
       <c r="P19" s="15">
         <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="Q19" s="16">
         <f t="shared" ref="Q19:Q26" si="8">SUM(M19:P19)</f>
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="R19" s="31"/>
       <c r="S19" s="39"/>
@@ -2085,7 +2087,7 @@
       <c r="AM19" s="22"/>
       <c r="AN19" s="22"/>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>13</v>
       </c>
@@ -2156,7 +2158,7 @@
       <c r="AM20" s="22"/>
       <c r="AN20" s="22"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>14</v>
       </c>
@@ -2225,8 +2227,8 @@
       <c r="AM21" s="22"/>
       <c r="AN21" s="22"/>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A22" s="49" t="s">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A22" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="25" t="s">
@@ -2294,7 +2296,7 @@
       <c r="AM22" s="22"/>
       <c r="AN22" s="22"/>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>16</v>
       </c>
@@ -2367,7 +2369,7 @@
       <c r="AM23" s="22"/>
       <c r="AN23" s="22"/>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>49</v>
       </c>
@@ -2436,7 +2438,7 @@
       <c r="AM24" s="22"/>
       <c r="AN24" s="22"/>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>50</v>
       </c>
@@ -2505,7 +2507,7 @@
       <c r="AM25" s="22"/>
       <c r="AN25" s="22"/>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>51</v>
       </c>
@@ -2574,7 +2576,7 @@
       <c r="AM26" s="22"/>
       <c r="AN26" s="22"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="25"/>
       <c r="C27" s="17"/>
@@ -2616,7 +2618,7 @@
       <c r="AM27" s="22"/>
       <c r="AN27" s="22"/>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>17</v>
       </c>
@@ -2665,7 +2667,7 @@
       <c r="AM28" s="22"/>
       <c r="AN28" s="22"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>18</v>
       </c>
@@ -2736,7 +2738,7 @@
       <c r="AM29" s="22"/>
       <c r="AN29" s="22"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>19</v>
       </c>
@@ -2805,7 +2807,7 @@
       <c r="AM30" s="22"/>
       <c r="AN30" s="22"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>20</v>
       </c>
@@ -2874,7 +2876,7 @@
       <c r="AM31" s="22"/>
       <c r="AN31" s="22"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>21</v>
       </c>
@@ -2945,7 +2947,7 @@
       <c r="AM32" s="22"/>
       <c r="AN32" s="22"/>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="18"/>
       <c r="B33" s="25"/>
       <c r="C33" s="17"/>
@@ -2990,7 +2992,7 @@
       <c r="AM33" s="22"/>
       <c r="AN33" s="22"/>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
         <v>22</v>
       </c>
@@ -3039,7 +3041,7 @@
       <c r="AM34" s="22"/>
       <c r="AN34" s="22"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>23</v>
       </c>
@@ -3114,7 +3116,7 @@
       <c r="AM35" s="22"/>
       <c r="AN35" s="22"/>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>24</v>
       </c>
@@ -3189,7 +3191,7 @@
       <c r="AM36" s="22"/>
       <c r="AN36" s="22"/>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
       <c r="B37" s="25"/>
       <c r="C37" s="17"/>
@@ -3231,7 +3233,7 @@
       <c r="AM37" s="22"/>
       <c r="AN37" s="22"/>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
         <v>25</v>
       </c>
@@ -3283,7 +3285,7 @@
       <c r="AM38" s="22"/>
       <c r="AN38" s="22"/>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
         <v>26</v>
       </c>
@@ -3358,7 +3360,7 @@
       <c r="AM39" s="22"/>
       <c r="AN39" s="22"/>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>27</v>
       </c>
@@ -3433,7 +3435,7 @@
       <c r="AM40" s="22"/>
       <c r="AN40" s="22"/>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="25"/>
       <c r="C41" s="17"/>
@@ -3475,7 +3477,7 @@
       <c r="AM41" s="22"/>
       <c r="AN41" s="22"/>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" s="24" t="s">
         <v>75</v>
       </c>
@@ -3524,7 +3526,7 @@
       <c r="AM42" s="22"/>
       <c r="AN42" s="22"/>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
         <v>76</v>
       </c>
@@ -3547,33 +3549,41 @@
         <f t="shared" ref="G43:G48" si="12">SUM(C43:F43)</f>
         <v>9</v>
       </c>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
+      <c r="H43" s="17">
+        <v>2</v>
+      </c>
+      <c r="I43" s="17">
+        <v>1</v>
+      </c>
+      <c r="J43" s="17">
+        <v>1</v>
+      </c>
+      <c r="K43" s="17">
+        <v>1</v>
+      </c>
       <c r="L43" s="9">
         <f>SUM(H43:K43)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M43" s="15">
         <f t="shared" ref="M43:P48" si="13">H43-C43</f>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="N43" s="15">
         <f t="shared" si="13"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="O43" s="15">
         <f t="shared" si="13"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="P43" s="15">
         <f t="shared" si="13"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Q43" s="16">
         <f t="shared" ref="Q43:Q48" si="14">SUM(M43:P43)</f>
-        <v>-9</v>
+        <v>-4</v>
       </c>
       <c r="R43" s="30"/>
       <c r="S43" s="30"/>
@@ -3599,7 +3609,7 @@
       <c r="AM43" s="22"/>
       <c r="AN43" s="22"/>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
         <v>77</v>
       </c>
@@ -3674,7 +3684,7 @@
       <c r="AM44" s="22"/>
       <c r="AN44" s="22"/>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
         <v>78</v>
       </c>
@@ -3707,11 +3717,11 @@
         <v>2</v>
       </c>
       <c r="K45" s="17">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L45" s="9">
         <f>SUM(H45:K45)</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="M45" s="15">
         <f t="shared" si="13"/>
@@ -3727,11 +3737,11 @@
       </c>
       <c r="P45" s="15">
         <f t="shared" si="13"/>
-        <v>-8</v>
+        <v>-7.5</v>
       </c>
       <c r="Q45" s="16">
         <f t="shared" si="14"/>
-        <v>-32</v>
+        <v>-31.5</v>
       </c>
       <c r="R45" s="30"/>
       <c r="S45" s="30"/>
@@ -3757,7 +3767,7 @@
       <c r="AM45" s="22"/>
       <c r="AN45" s="22"/>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
         <v>79</v>
       </c>
@@ -3780,33 +3790,41 @@
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
+      <c r="H46" s="17">
+        <v>2</v>
+      </c>
+      <c r="I46" s="17">
+        <v>1</v>
+      </c>
+      <c r="J46" s="17">
+        <v>1</v>
+      </c>
+      <c r="K46" s="17">
+        <v>1</v>
+      </c>
       <c r="L46" s="9">
         <f>SUM(H46:K46)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M46" s="15">
         <f t="shared" si="13"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="N46" s="15">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O46" s="15">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P46" s="15">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="16">
         <f t="shared" si="14"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="R46" s="22"/>
       <c r="S46" s="30"/>
@@ -3832,7 +3850,7 @@
       <c r="AM46" s="22"/>
       <c r="AN46" s="22"/>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
         <v>80</v>
       </c>
@@ -3904,7 +3922,7 @@
       <c r="AM47" s="22"/>
       <c r="AN47" s="22"/>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
         <v>81</v>
       </c>
@@ -3979,7 +3997,7 @@
       <c r="AM48" s="22"/>
       <c r="AN48" s="22"/>
     </row>
-    <row r="49" spans="2:17" s="11" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:17" s="11" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
         <v>3</v>
       </c>
@@ -4005,97 +4023,97 @@
       </c>
       <c r="H49" s="13">
         <f t="shared" ref="H49:Q49" si="15">SUM(H10:H48)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I49" s="13">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J49" s="13">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K49" s="13">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>11.5</v>
       </c>
       <c r="L49" s="20">
         <f t="shared" si="15"/>
-        <v>35</v>
+        <v>46.5</v>
       </c>
       <c r="M49" s="13">
         <f t="shared" si="15"/>
-        <v>-101</v>
+        <v>-97</v>
       </c>
       <c r="N49" s="13">
         <f t="shared" si="15"/>
-        <v>-94</v>
+        <v>-92</v>
       </c>
       <c r="O49" s="13">
         <f t="shared" si="15"/>
-        <v>-105</v>
+        <v>-103</v>
       </c>
       <c r="P49" s="13">
         <f t="shared" si="15"/>
-        <v>-101</v>
+        <v>-97.5</v>
       </c>
       <c r="Q49" s="21">
         <f t="shared" si="15"/>
-        <v>-401</v>
-      </c>
-    </row>
-    <row r="50" spans="2:17" ht="12" thickTop="1" x14ac:dyDescent="0.15"/>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.15">
+        <v>-389.5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B52" s="37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B53" s="36" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B54" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B55" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B56" s="34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>89</v>
       </c>
@@ -4127,7 +4145,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
@@ -4140,7 +4158,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>

<commit_message>
Stunden eingetragen in den Projektplan und Zeitblatt
</commit_message>
<xml_diff>
--- a/Projekt Handbuch/Projektplan.xlsx
+++ b/Projekt Handbuch/Projektplan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
-  <workbookPr checkCompatibility="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ursus/Git/AlienHacky/Projekt Handbuch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Documents\AlienSoccer\Projekt Handbuch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <author>Stefan Hagen</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP13" authorId="0">
+    <comment ref="AP13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>Aufwand IST</t>
   </si>
@@ -357,11 +357,17 @@
   <si>
     <t xml:space="preserve">    AlienServer: Komm DMX, Zigbee</t>
   </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Grundgerüst</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0_ ;[Red]\-0.0\ "/>
   </numFmts>
@@ -422,6 +428,7 @@
       <i/>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -434,12 +441,14 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -594,7 +603,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -695,6 +704,9 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -716,14 +728,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1191,109 +1207,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AP64"/>
+  <dimension ref="A1:AP65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="Q38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="9" topLeftCell="H31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B60" sqref="B60:B64"/>
+      <selection pane="bottomRight" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" customWidth="1"/>
     <col min="3" max="6" width="4" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="4" style="1" customWidth="1"/>
-    <col min="13" max="17" width="5.5" style="1" customWidth="1"/>
-    <col min="18" max="40" width="3.6640625" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="11.5" style="1"/>
+    <col min="13" max="17" width="5.42578125" style="1" customWidth="1"/>
+    <col min="18" max="40" width="3.7109375" style="1" customWidth="1"/>
+    <col min="41" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:42" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="42" t="s">
+    <row r="8" spans="1:42" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="47" t="s">
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="46">
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="47">
         <v>2016</v>
       </c>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="46"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="46"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="46">
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="47"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="47"/>
+      <c r="AE8" s="47"/>
+      <c r="AF8" s="47">
         <v>2017</v>
       </c>
-      <c r="AG8" s="46"/>
-      <c r="AH8" s="46"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="46"/>
-      <c r="AK8" s="46"/>
-      <c r="AL8" s="46"/>
-      <c r="AM8" s="46"/>
-      <c r="AN8" s="46"/>
-    </row>
-    <row r="9" spans="1:42" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="44"/>
-      <c r="B9" s="43"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="47"/>
+      <c r="AJ8" s="47"/>
+      <c r="AK8" s="47"/>
+      <c r="AL8" s="47"/>
+      <c r="AM8" s="47"/>
+      <c r="AN8" s="47"/>
+    </row>
+    <row r="9" spans="1:42" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="45"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1425,7 +1441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>5</v>
       </c>
@@ -1474,7 +1490,7 @@
       <c r="AM10" s="22"/>
       <c r="AN10" s="22"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>7</v>
       </c>
@@ -1504,14 +1520,14 @@
         <v>4</v>
       </c>
       <c r="J11" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K11" s="17">
         <v>4</v>
       </c>
       <c r="L11" s="9">
         <f t="shared" ref="L11:L16" si="2">SUM(H11:K11)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M11" s="15">
         <f t="shared" ref="M11:P16" si="3">H11-C11</f>
@@ -1523,7 +1539,7 @@
       </c>
       <c r="O11" s="15">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="P11" s="15">
         <f t="shared" si="3"/>
@@ -1531,7 +1547,7 @@
       </c>
       <c r="Q11" s="16">
         <f t="shared" ref="Q11:Q16" si="4">SUM(M11:P11)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="R11" s="30"/>
       <c r="S11" s="30"/>
@@ -1557,7 +1573,7 @@
       <c r="AM11" s="22"/>
       <c r="AN11" s="22"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>6</v>
       </c>
@@ -1581,12 +1597,16 @@
         <v>16</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+      <c r="I12" s="17">
+        <v>2</v>
+      </c>
+      <c r="J12" s="17">
+        <v>2</v>
+      </c>
       <c r="K12" s="17"/>
       <c r="L12" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="3"/>
@@ -1594,11 +1614,11 @@
       </c>
       <c r="N12" s="15">
         <f t="shared" si="3"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="O12" s="15">
         <f t="shared" si="3"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="P12" s="15">
         <f t="shared" si="3"/>
@@ -1606,7 +1626,7 @@
       </c>
       <c r="Q12" s="16">
         <f t="shared" si="4"/>
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="R12" s="30"/>
       <c r="S12" s="30"/>
@@ -1632,7 +1652,7 @@
       <c r="AM12" s="22"/>
       <c r="AN12" s="22"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>8</v>
       </c>
@@ -1710,7 +1730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
@@ -1789,7 +1809,7 @@
       <c r="AM14" s="22"/>
       <c r="AN14" s="22"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
@@ -1872,7 +1892,7 @@
       <c r="AM15" s="22"/>
       <c r="AN15" s="22"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>70</v>
       </c>
@@ -1941,7 +1961,7 @@
       <c r="AM16" s="22"/>
       <c r="AN16" s="22"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="25"/>
       <c r="C17" s="17"/>
@@ -1983,7 +2003,7 @@
       <c r="AM17" s="22"/>
       <c r="AN17" s="22"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>11</v>
       </c>
@@ -2032,7 +2052,7 @@
       <c r="AM18" s="22"/>
       <c r="AN18" s="22"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
@@ -2103,7 +2123,7 @@
       <c r="AM19" s="22"/>
       <c r="AN19" s="22"/>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>13</v>
       </c>
@@ -2122,13 +2142,15 @@
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17">
-        <v>8</v>
-      </c>
-      <c r="J20" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="J20" s="17">
+        <v>1</v>
+      </c>
       <c r="K20" s="17"/>
       <c r="L20" s="9">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M20" s="15">
         <f t="shared" si="7"/>
@@ -2136,11 +2158,11 @@
       </c>
       <c r="N20" s="15">
         <f t="shared" si="7"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="O20" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="15">
         <f t="shared" si="7"/>
@@ -2148,7 +2170,7 @@
       </c>
       <c r="Q20" s="16">
         <f t="shared" si="8"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="R20" s="40"/>
       <c r="S20" s="40"/>
@@ -2174,7 +2196,7 @@
       <c r="AM20" s="22"/>
       <c r="AN20" s="22"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>14</v>
       </c>
@@ -2192,12 +2214,14 @@
         <v>10</v>
       </c>
       <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="I21" s="17">
+        <v>5</v>
+      </c>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
       <c r="L21" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M21" s="15">
         <f t="shared" si="7"/>
@@ -2205,7 +2229,7 @@
       </c>
       <c r="N21" s="15">
         <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="O21" s="15">
         <f t="shared" si="7"/>
@@ -2217,7 +2241,7 @@
       </c>
       <c r="Q21" s="16">
         <f t="shared" si="8"/>
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="R21" s="23"/>
       <c r="S21" s="23"/>
@@ -2243,8 +2267,8 @@
       <c r="AM21" s="22"/>
       <c r="AN21" s="22"/>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A22" s="49" t="s">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A22" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="25" t="s">
@@ -2312,7 +2336,7 @@
       <c r="AM22" s="22"/>
       <c r="AN22" s="22"/>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>16</v>
       </c>
@@ -2334,12 +2358,14 @@
         <v>22</v>
       </c>
       <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+      <c r="I23" s="17">
+        <v>6</v>
+      </c>
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
       <c r="L23" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M23" s="15">
         <f t="shared" si="7"/>
@@ -2347,7 +2373,7 @@
       </c>
       <c r="N23" s="15">
         <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>-4</v>
       </c>
       <c r="O23" s="15">
         <f t="shared" si="7"/>
@@ -2359,7 +2385,7 @@
       </c>
       <c r="Q23" s="16">
         <f t="shared" si="8"/>
-        <v>-22</v>
+        <v>-16</v>
       </c>
       <c r="R23" s="23"/>
       <c r="S23" s="23"/>
@@ -2385,7 +2411,7 @@
       <c r="AM23" s="22"/>
       <c r="AN23" s="22"/>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>49</v>
       </c>
@@ -2404,11 +2430,14 @@
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
+      <c r="J24" s="17">
+        <f>7+2+1+1.5+3.5</f>
+        <v>15</v>
+      </c>
       <c r="K24" s="17"/>
       <c r="L24" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M24" s="15">
         <f t="shared" si="7"/>
@@ -2420,7 +2449,7 @@
       </c>
       <c r="O24" s="15">
         <f t="shared" si="7"/>
-        <v>-14</v>
+        <v>1</v>
       </c>
       <c r="P24" s="15">
         <f t="shared" si="7"/>
@@ -2428,7 +2457,7 @@
       </c>
       <c r="Q24" s="16">
         <f t="shared" si="8"/>
-        <v>-14</v>
+        <v>1</v>
       </c>
       <c r="R24" s="41"/>
       <c r="S24" s="41"/>
@@ -2454,7 +2483,7 @@
       <c r="AM24" s="22"/>
       <c r="AN24" s="22"/>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>50</v>
       </c>
@@ -2523,7 +2552,7 @@
       <c r="AM25" s="22"/>
       <c r="AN25" s="22"/>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>51</v>
       </c>
@@ -2592,7 +2621,7 @@
       <c r="AM26" s="22"/>
       <c r="AN26" s="22"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="25"/>
       <c r="C27" s="17"/>
@@ -2634,7 +2663,7 @@
       <c r="AM27" s="22"/>
       <c r="AN27" s="22"/>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>17</v>
       </c>
@@ -2647,7 +2676,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="32">
         <f>SUM(G29:G32)</f>
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
@@ -2683,7 +2712,7 @@
       <c r="AM28" s="22"/>
       <c r="AN28" s="22"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>18</v>
       </c>
@@ -2754,7 +2783,7 @@
       <c r="AM29" s="22"/>
       <c r="AN29" s="22"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>19</v>
       </c>
@@ -2823,7 +2852,7 @@
       <c r="AM30" s="22"/>
       <c r="AN30" s="22"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>20</v>
       </c>
@@ -2833,12 +2862,12 @@
       <c r="C31" s="29"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="10">
         <f>SUM(C31:F31)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
@@ -2858,7 +2887,7 @@
       </c>
       <c r="O31" s="15">
         <f t="shared" si="9"/>
-        <v>-20</v>
+        <v>-18</v>
       </c>
       <c r="P31" s="15">
         <f t="shared" si="9"/>
@@ -2866,7 +2895,7 @@
       </c>
       <c r="Q31" s="16">
         <f>SUM(M31:P31)</f>
-        <v>-20</v>
+        <v>-18</v>
       </c>
       <c r="R31" s="23"/>
       <c r="S31" s="41"/>
@@ -2892,7 +2921,7 @@
       <c r="AM31" s="22"/>
       <c r="AN31" s="22"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>21</v>
       </c>
@@ -2963,39 +2992,65 @@
       <c r="AM32" s="22"/>
       <c r="AN32" s="22"/>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A33" s="18"/>
-      <c r="B33" s="25"/>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A33" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>94</v>
+      </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
+      <c r="E33" s="17">
+        <v>2</v>
+      </c>
       <c r="F33" s="17"/>
-      <c r="G33" s="10"/>
+      <c r="G33" s="10">
+        <f>C33+D33+E33+F33</f>
+        <v>2</v>
+      </c>
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
+      <c r="J33" s="17">
+        <v>2</v>
+      </c>
       <c r="K33" s="17"/>
       <c r="L33" s="9">
         <f>SUM(H33:K33)</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="M33" s="15">
+        <f t="shared" ref="M33" si="10">H33-C33</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="15">
+        <f t="shared" ref="N33" si="11">I33-D33</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="15">
+        <f t="shared" ref="O33" si="12">J33-E33</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="15">
+        <f t="shared" ref="P33" si="13">K33-F33</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="16">
+        <f>SUM(M33:P33)</f>
+        <v>0</v>
+      </c>
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
-      <c r="U33" s="22"/>
-      <c r="V33" s="22"/>
-      <c r="W33" s="22"/>
-      <c r="X33" s="22"/>
-      <c r="Y33" s="22"/>
-      <c r="Z33" s="22"/>
-      <c r="AA33" s="22"/>
-      <c r="AB33" s="22"/>
-      <c r="AC33" s="22"/>
+      <c r="U33" s="52"/>
+      <c r="V33" s="23"/>
+      <c r="W33" s="31"/>
+      <c r="X33" s="31"/>
+      <c r="Y33" s="51"/>
+      <c r="Z33" s="51"/>
+      <c r="AA33" s="51"/>
+      <c r="AB33" s="51"/>
+      <c r="AC33" s="31"/>
       <c r="AD33" s="26"/>
       <c r="AE33" s="26"/>
       <c r="AF33" s="26"/>
@@ -3008,21 +3063,14 @@
       <c r="AM33" s="22"/>
       <c r="AN33" s="22"/>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A34" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>41</v>
-      </c>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="32">
-        <f>SUM(G35:G36)</f>
-        <v>32</v>
-      </c>
+      <c r="G34" s="10"/>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
@@ -3057,62 +3105,36 @@
       <c r="AM34" s="22"/>
       <c r="AN34" s="22"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A35" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="17">
-        <v>4</v>
-      </c>
-      <c r="D35" s="17">
-        <v>4</v>
-      </c>
-      <c r="E35" s="17">
-        <v>4</v>
-      </c>
-      <c r="F35" s="17">
-        <v>4</v>
-      </c>
-      <c r="G35" s="10">
-        <f>SUM(C35:F35)</f>
-        <v>16</v>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A35" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="32">
+        <f>SUM(G36:G37)</f>
+        <v>32</v>
       </c>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
-      <c r="L35" s="9">
-        <f>SUM(H35:K35)</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="15">
-        <f t="shared" ref="M35:P36" si="10">H35-C35</f>
-        <v>-4</v>
-      </c>
-      <c r="N35" s="15">
-        <f t="shared" si="10"/>
-        <v>-4</v>
-      </c>
-      <c r="O35" s="15">
-        <f t="shared" si="10"/>
-        <v>-4</v>
-      </c>
-      <c r="P35" s="15">
-        <f t="shared" si="10"/>
-        <v>-4</v>
-      </c>
-      <c r="Q35" s="16">
-        <f>SUM(M35:P35)</f>
-        <v>-16</v>
-      </c>
+      <c r="L35" s="9"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="16"/>
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="22"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
       <c r="W35" s="22"/>
       <c r="X35" s="22"/>
       <c r="Y35" s="22"/>
@@ -3132,12 +3154,12 @@
       <c r="AM35" s="22"/>
       <c r="AN35" s="22"/>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" s="17">
         <v>4</v>
@@ -3155,33 +3177,41 @@
         <f>SUM(C36:F36)</f>
         <v>16</v>
       </c>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
+      <c r="H36" s="17">
+        <v>2</v>
+      </c>
+      <c r="I36" s="17">
+        <v>2</v>
+      </c>
+      <c r="J36" s="17">
+        <v>2</v>
+      </c>
+      <c r="K36" s="17">
+        <v>2</v>
+      </c>
       <c r="L36" s="9">
         <f>SUM(H36:K36)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M36" s="15">
-        <f t="shared" si="10"/>
-        <v>-4</v>
+        <f t="shared" ref="M36:P37" si="14">H36-C36</f>
+        <v>-2</v>
       </c>
       <c r="N36" s="15">
-        <f t="shared" si="10"/>
-        <v>-4</v>
+        <f t="shared" si="14"/>
+        <v>-2</v>
       </c>
       <c r="O36" s="15">
-        <f t="shared" si="10"/>
-        <v>-4</v>
+        <f t="shared" si="14"/>
+        <v>-2</v>
       </c>
       <c r="P36" s="15">
-        <f t="shared" si="10"/>
-        <v>-4</v>
+        <f t="shared" si="14"/>
+        <v>-2</v>
       </c>
       <c r="Q36" s="16">
         <f>SUM(M36:P36)</f>
-        <v>-16</v>
+        <v>-8</v>
       </c>
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
@@ -3207,29 +3237,70 @@
       <c r="AM36" s="22"/>
       <c r="AN36" s="22"/>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A37" s="18"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="16"/>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="17">
+        <v>4</v>
+      </c>
+      <c r="D37" s="17">
+        <v>4</v>
+      </c>
+      <c r="E37" s="17">
+        <v>4</v>
+      </c>
+      <c r="F37" s="17">
+        <v>4</v>
+      </c>
+      <c r="G37" s="10">
+        <f>SUM(C37:F37)</f>
+        <v>16</v>
+      </c>
+      <c r="H37" s="17">
+        <v>2</v>
+      </c>
+      <c r="I37" s="17">
+        <v>2</v>
+      </c>
+      <c r="J37" s="17">
+        <v>2</v>
+      </c>
+      <c r="K37" s="17">
+        <v>2</v>
+      </c>
+      <c r="L37" s="9">
+        <f>SUM(H37:K37)</f>
+        <v>8</v>
+      </c>
+      <c r="M37" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="N37" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="O37" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="P37" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="Q37" s="16">
+        <f>SUM(M37:P37)</f>
+        <v>-8</v>
+      </c>
       <c r="R37" s="22"/>
       <c r="S37" s="22"/>
       <c r="T37" s="22"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
+      <c r="U37" s="30"/>
+      <c r="V37" s="30"/>
       <c r="W37" s="22"/>
       <c r="X37" s="22"/>
       <c r="Y37" s="22"/>
@@ -3249,29 +3320,19 @@
       <c r="AM37" s="22"/>
       <c r="AN37" s="22"/>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A38" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>71</v>
-      </c>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A38" s="18"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
-      <c r="G38" s="32">
-        <f>SUM(G39:G40)</f>
-        <v>48</v>
-      </c>
+      <c r="G38" s="10"/>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
-      <c r="L38" s="9">
-        <f>SUM(H38:K38)</f>
-        <v>0</v>
-      </c>
+      <c r="L38" s="9"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -3280,8 +3341,8 @@
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
-      <c r="V38" s="22"/>
+      <c r="U38" s="23"/>
+      <c r="V38" s="23"/>
       <c r="W38" s="22"/>
       <c r="X38" s="22"/>
       <c r="Y38" s="22"/>
@@ -3301,28 +3362,20 @@
       <c r="AM38" s="22"/>
       <c r="AN38" s="22"/>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A39" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="17">
-        <v>10</v>
-      </c>
-      <c r="D39" s="17">
-        <v>10</v>
-      </c>
-      <c r="E39" s="17">
-        <v>10</v>
-      </c>
-      <c r="F39" s="17">
-        <v>10</v>
-      </c>
-      <c r="G39" s="10">
-        <f>SUM(C39:F39)</f>
-        <v>40</v>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A39" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="32">
+        <f>SUM(G40:G41)</f>
+        <v>48</v>
       </c>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
@@ -3332,38 +3385,23 @@
         <f>SUM(H39:K39)</f>
         <v>0</v>
       </c>
-      <c r="M39" s="15">
-        <f t="shared" ref="M39:P40" si="11">H39-C39</f>
-        <v>-10</v>
-      </c>
-      <c r="N39" s="15">
-        <f t="shared" si="11"/>
-        <v>-10</v>
-      </c>
-      <c r="O39" s="15">
-        <f t="shared" si="11"/>
-        <v>-10</v>
-      </c>
-      <c r="P39" s="15">
-        <f t="shared" si="11"/>
-        <v>-10</v>
-      </c>
-      <c r="Q39" s="16">
-        <f>SUM(M39:P39)</f>
-        <v>-40</v>
-      </c>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="16"/>
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="23"/>
-      <c r="V39" s="30"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="30"/>
-      <c r="AC39" s="30"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="22"/>
+      <c r="X39" s="22"/>
+      <c r="Y39" s="22"/>
+      <c r="Z39" s="22"/>
+      <c r="AA39" s="22"/>
+      <c r="AB39" s="22"/>
+      <c r="AC39" s="22"/>
       <c r="AD39" s="26"/>
       <c r="AE39" s="26"/>
       <c r="AF39" s="26"/>
@@ -3376,28 +3414,28 @@
       <c r="AM39" s="22"/>
       <c r="AN39" s="22"/>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C40" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D40" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E40" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F40" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G40" s="10">
         <f>SUM(C40:F40)</f>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
@@ -3408,24 +3446,24 @@
         <v>0</v>
       </c>
       <c r="M40" s="15">
-        <f t="shared" si="11"/>
-        <v>-2</v>
+        <f t="shared" ref="M40:P41" si="15">H40-C40</f>
+        <v>-10</v>
       </c>
       <c r="N40" s="15">
-        <f t="shared" si="11"/>
-        <v>-2</v>
+        <f t="shared" si="15"/>
+        <v>-10</v>
       </c>
       <c r="O40" s="15">
-        <f t="shared" si="11"/>
-        <v>-2</v>
+        <f t="shared" si="15"/>
+        <v>-10</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" si="11"/>
-        <v>-2</v>
+        <f t="shared" si="15"/>
+        <v>-10</v>
       </c>
       <c r="Q40" s="16">
         <f>SUM(M40:P40)</f>
-        <v>-8</v>
+        <v>-40</v>
       </c>
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
@@ -3451,24 +3489,57 @@
       <c r="AM40" s="22"/>
       <c r="AN40" s="22"/>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A41" s="18"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="10"/>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="17">
+        <v>2</v>
+      </c>
+      <c r="D41" s="17">
+        <v>2</v>
+      </c>
+      <c r="E41" s="17">
+        <v>2</v>
+      </c>
+      <c r="F41" s="17">
+        <v>2</v>
+      </c>
+      <c r="G41" s="10">
+        <f>SUM(C41:F41)</f>
+        <v>8</v>
+      </c>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="16"/>
+      <c r="L41" s="9">
+        <f>SUM(H41:K41)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="N41" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="O41" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="P41" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="Q41" s="16">
+        <f>SUM(M41:P41)</f>
+        <v>-8</v>
+      </c>
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
       <c r="T41" s="23"/>
@@ -3493,21 +3564,14 @@
       <c r="AM41" s="22"/>
       <c r="AN41" s="22"/>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A42" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>44</v>
-      </c>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A42" s="18"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="32">
-        <f>SUM(G43:G48)</f>
-        <v>106</v>
-      </c>
+      <c r="G42" s="10"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
@@ -3520,16 +3584,16 @@
       <c r="Q42" s="16"/>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
-      <c r="T42" s="22"/>
-      <c r="U42" s="22"/>
-      <c r="V42" s="22"/>
-      <c r="W42" s="22"/>
-      <c r="X42" s="22"/>
-      <c r="Y42" s="22"/>
-      <c r="Z42" s="22"/>
-      <c r="AA42" s="22"/>
-      <c r="AB42" s="22"/>
-      <c r="AC42" s="22"/>
+      <c r="T42" s="23"/>
+      <c r="U42" s="23"/>
+      <c r="V42" s="30"/>
+      <c r="W42" s="30"/>
+      <c r="X42" s="30"/>
+      <c r="Y42" s="30"/>
+      <c r="Z42" s="30"/>
+      <c r="AA42" s="30"/>
+      <c r="AB42" s="30"/>
+      <c r="AC42" s="30"/>
       <c r="AD42" s="26"/>
       <c r="AE42" s="26"/>
       <c r="AF42" s="26"/>
@@ -3542,68 +3606,34 @@
       <c r="AM42" s="22"/>
       <c r="AN42" s="22"/>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A43" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="17">
-        <v>3</v>
-      </c>
-      <c r="D43" s="17">
-        <v>2</v>
-      </c>
-      <c r="E43" s="17">
-        <v>2</v>
-      </c>
-      <c r="F43" s="17">
-        <v>2</v>
-      </c>
-      <c r="G43" s="10">
-        <f t="shared" ref="G43:G48" si="12">SUM(C43:F43)</f>
-        <v>9</v>
-      </c>
-      <c r="H43" s="17">
-        <v>2</v>
-      </c>
-      <c r="I43" s="17">
-        <v>1</v>
-      </c>
-      <c r="J43" s="17">
-        <v>1</v>
-      </c>
-      <c r="K43" s="17">
-        <v>1</v>
-      </c>
-      <c r="L43" s="9">
-        <f>SUM(H43:K43)</f>
-        <v>5</v>
-      </c>
-      <c r="M43" s="15">
-        <f t="shared" ref="M43:P48" si="13">H43-C43</f>
-        <v>-1</v>
-      </c>
-      <c r="N43" s="15">
-        <f t="shared" si="13"/>
-        <v>-1</v>
-      </c>
-      <c r="O43" s="15">
-        <f t="shared" si="13"/>
-        <v>-1</v>
-      </c>
-      <c r="P43" s="15">
-        <f t="shared" si="13"/>
-        <v>-1</v>
-      </c>
-      <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q48" si="14">SUM(M43:P43)</f>
-        <v>-4</v>
-      </c>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="32">
+        <f>SUM(G44:G49)</f>
+        <v>106</v>
+      </c>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
       <c r="U43" s="22"/>
       <c r="V43" s="22"/>
       <c r="W43" s="22"/>
@@ -3625,69 +3655,77 @@
       <c r="AM43" s="22"/>
       <c r="AN43" s="22"/>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C44" s="17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D44" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E44" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F44" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G44" s="10">
-        <f t="shared" si="12"/>
-        <v>24</v>
-      </c>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="17"/>
+        <f t="shared" ref="G44:G49" si="16">SUM(C44:F44)</f>
+        <v>9</v>
+      </c>
+      <c r="H44" s="17">
+        <v>2</v>
+      </c>
+      <c r="I44" s="17">
+        <v>1</v>
+      </c>
+      <c r="J44" s="17">
+        <v>1</v>
+      </c>
+      <c r="K44" s="17">
+        <v>1</v>
+      </c>
       <c r="L44" s="9">
         <f>SUM(H44:K44)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M44" s="15">
-        <f t="shared" si="13"/>
-        <v>-6</v>
+        <f t="shared" ref="M44:P49" si="17">H44-C44</f>
+        <v>-1</v>
       </c>
       <c r="N44" s="15">
-        <f t="shared" si="13"/>
-        <v>-6</v>
+        <f t="shared" si="17"/>
+        <v>-1</v>
       </c>
       <c r="O44" s="15">
-        <f t="shared" si="13"/>
-        <v>-6</v>
+        <f t="shared" si="17"/>
+        <v>-1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" si="13"/>
-        <v>-6</v>
+        <f t="shared" si="17"/>
+        <v>-1</v>
       </c>
       <c r="Q44" s="16">
-        <f t="shared" si="14"/>
-        <v>-24</v>
-      </c>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
+        <f t="shared" ref="Q44:Q49" si="18">SUM(M44:P44)</f>
+        <v>-4</v>
+      </c>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+      <c r="T44" s="30"/>
       <c r="U44" s="22"/>
       <c r="V44" s="22"/>
       <c r="W44" s="22"/>
       <c r="X44" s="22"/>
       <c r="Y44" s="22"/>
-      <c r="Z44" s="30"/>
-      <c r="AA44" s="30"/>
-      <c r="AB44" s="30"/>
-      <c r="AC44" s="30"/>
+      <c r="Z44" s="22"/>
+      <c r="AA44" s="22"/>
+      <c r="AB44" s="22"/>
+      <c r="AC44" s="22"/>
       <c r="AD44" s="26"/>
       <c r="AE44" s="26"/>
       <c r="AF44" s="26"/>
@@ -3700,73 +3738,65 @@
       <c r="AM44" s="22"/>
       <c r="AN44" s="22"/>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C45" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D45" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E45" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F45" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G45" s="10">
-        <f t="shared" si="12"/>
-        <v>40</v>
-      </c>
-      <c r="H45" s="17">
-        <v>2</v>
-      </c>
-      <c r="I45" s="17">
-        <v>2</v>
-      </c>
-      <c r="J45" s="17">
-        <v>2</v>
-      </c>
-      <c r="K45" s="17">
-        <v>2.5</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>24</v>
+      </c>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
       <c r="L45" s="9">
         <f>SUM(H45:K45)</f>
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="M45" s="15">
-        <f t="shared" si="13"/>
-        <v>-8</v>
+        <f t="shared" si="17"/>
+        <v>-6</v>
       </c>
       <c r="N45" s="15">
-        <f t="shared" si="13"/>
-        <v>-8</v>
+        <f t="shared" si="17"/>
+        <v>-6</v>
       </c>
       <c r="O45" s="15">
-        <f t="shared" si="13"/>
-        <v>-8</v>
+        <f t="shared" si="17"/>
+        <v>-6</v>
       </c>
       <c r="P45" s="15">
-        <f t="shared" si="13"/>
-        <v>-7.5</v>
+        <f t="shared" si="17"/>
+        <v>-6</v>
       </c>
       <c r="Q45" s="16">
-        <f t="shared" si="14"/>
-        <v>-31.5</v>
-      </c>
-      <c r="R45" s="30"/>
-      <c r="S45" s="30"/>
-      <c r="T45" s="30"/>
-      <c r="U45" s="30"/>
-      <c r="V45" s="30"/>
-      <c r="W45" s="30"/>
-      <c r="X45" s="30"/>
-      <c r="Y45" s="30"/>
+        <f t="shared" si="18"/>
+        <v>-24</v>
+      </c>
+      <c r="R45" s="22"/>
+      <c r="S45" s="22"/>
+      <c r="T45" s="22"/>
+      <c r="U45" s="22"/>
+      <c r="V45" s="22"/>
+      <c r="W45" s="22"/>
+      <c r="X45" s="22"/>
+      <c r="Y45" s="22"/>
       <c r="Z45" s="30"/>
       <c r="AA45" s="30"/>
       <c r="AB45" s="30"/>
@@ -3783,77 +3813,77 @@
       <c r="AM45" s="22"/>
       <c r="AN45" s="22"/>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C46" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D46" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E46" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F46" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G46" s="10">
-        <f t="shared" si="12"/>
-        <v>5</v>
+        <f t="shared" si="16"/>
+        <v>40</v>
       </c>
       <c r="H46" s="17">
         <v>2</v>
       </c>
       <c r="I46" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J46" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K46" s="17">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="L46" s="9">
         <f>SUM(H46:K46)</f>
-        <v>5</v>
+        <v>12.5</v>
       </c>
       <c r="M46" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>-8</v>
       </c>
       <c r="N46" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>-6</v>
       </c>
       <c r="O46" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>-6</v>
       </c>
       <c r="P46" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>-7.5</v>
       </c>
       <c r="Q46" s="16">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="R46" s="22"/>
+        <f t="shared" si="18"/>
+        <v>-27.5</v>
+      </c>
+      <c r="R46" s="30"/>
       <c r="S46" s="30"/>
-      <c r="T46" s="22"/>
-      <c r="U46" s="22"/>
-      <c r="V46" s="22"/>
-      <c r="W46" s="22"/>
-      <c r="X46" s="22"/>
-      <c r="Y46" s="22"/>
-      <c r="Z46" s="22"/>
-      <c r="AA46" s="22"/>
-      <c r="AB46" s="22"/>
-      <c r="AC46" s="22"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="30"/>
+      <c r="V46" s="30"/>
+      <c r="W46" s="30"/>
+      <c r="X46" s="30"/>
+      <c r="Y46" s="30"/>
+      <c r="Z46" s="30"/>
+      <c r="AA46" s="30"/>
+      <c r="AB46" s="30"/>
+      <c r="AC46" s="30"/>
       <c r="AD46" s="26"/>
       <c r="AE46" s="26"/>
       <c r="AF46" s="26"/>
@@ -3866,59 +3896,70 @@
       <c r="AM46" s="22"/>
       <c r="AN46" s="22"/>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D47" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" s="10">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="9"/>
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="H47" s="17">
+        <v>2</v>
+      </c>
+      <c r="I47" s="17">
+        <v>1</v>
+      </c>
+      <c r="J47" s="17">
+        <v>1</v>
+      </c>
+      <c r="K47" s="17">
+        <v>1</v>
+      </c>
+      <c r="L47" s="9">
+        <f>SUM(H47:K47)</f>
+        <v>5</v>
+      </c>
       <c r="M47" s="15">
-        <f t="shared" si="13"/>
-        <v>-4</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="N47" s="15">
-        <f t="shared" si="13"/>
-        <v>-2</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="O47" s="15">
-        <f t="shared" si="13"/>
-        <v>-2</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="P47" s="15">
-        <f t="shared" si="13"/>
-        <v>-2</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" si="14"/>
-        <v>-10</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="R47" s="22"/>
-      <c r="S47" s="22"/>
+      <c r="S47" s="30"/>
       <c r="T47" s="22"/>
       <c r="U47" s="22"/>
-      <c r="V47" s="30"/>
+      <c r="V47" s="22"/>
       <c r="W47" s="22"/>
       <c r="X47" s="22"/>
       <c r="Y47" s="22"/>
@@ -3938,62 +3979,70 @@
       <c r="AM47" s="22"/>
       <c r="AN47" s="22"/>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" s="17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D48" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E48" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F48" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G48" s="10">
-        <f t="shared" si="12"/>
-        <v>18</v>
-      </c>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="H48" s="17">
+        <v>3</v>
+      </c>
+      <c r="I48" s="17">
+        <v>3</v>
+      </c>
+      <c r="J48" s="17">
+        <v>3</v>
+      </c>
+      <c r="K48" s="17">
+        <v>3</v>
+      </c>
       <c r="L48" s="9">
         <f>SUM(H48:K48)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M48" s="15">
-        <f t="shared" si="13"/>
-        <v>-6</v>
+        <f t="shared" si="17"/>
+        <v>-1</v>
       </c>
       <c r="N48" s="15">
-        <f t="shared" si="13"/>
-        <v>-4</v>
+        <f t="shared" si="17"/>
+        <v>1</v>
       </c>
       <c r="O48" s="15">
-        <f t="shared" si="13"/>
-        <v>-4</v>
+        <f t="shared" si="17"/>
+        <v>1</v>
       </c>
       <c r="P48" s="15">
-        <f t="shared" si="13"/>
-        <v>-4</v>
+        <f t="shared" si="17"/>
+        <v>1</v>
       </c>
       <c r="Q48" s="16">
-        <f t="shared" si="14"/>
-        <v>-18</v>
+        <f t="shared" si="18"/>
+        <v>2</v>
       </c>
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
       <c r="T48" s="22"/>
       <c r="U48" s="22"/>
-      <c r="V48" s="22"/>
+      <c r="V48" s="30"/>
       <c r="W48" s="22"/>
       <c r="X48" s="22"/>
       <c r="Y48" s="22"/>
@@ -4004,7 +4053,7 @@
       <c r="AD48" s="26"/>
       <c r="AE48" s="26"/>
       <c r="AF48" s="26"/>
-      <c r="AG48" s="30"/>
+      <c r="AG48" s="22"/>
       <c r="AH48" s="22"/>
       <c r="AI48" s="22"/>
       <c r="AJ48" s="22"/>
@@ -4013,124 +4062,199 @@
       <c r="AM48" s="22"/>
       <c r="AN48" s="22"/>
     </row>
-    <row r="49" spans="2:17" s="11" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="12" t="s">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="17">
+        <v>6</v>
+      </c>
+      <c r="D49" s="17">
+        <v>4</v>
+      </c>
+      <c r="E49" s="17">
+        <v>4</v>
+      </c>
+      <c r="F49" s="17">
+        <v>4</v>
+      </c>
+      <c r="G49" s="10">
+        <f t="shared" si="16"/>
+        <v>18</v>
+      </c>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="9">
+        <f>SUM(H49:K49)</f>
+        <v>0</v>
+      </c>
+      <c r="M49" s="15">
+        <f t="shared" si="17"/>
+        <v>-6</v>
+      </c>
+      <c r="N49" s="15">
+        <f t="shared" si="17"/>
+        <v>-4</v>
+      </c>
+      <c r="O49" s="15">
+        <f t="shared" si="17"/>
+        <v>-4</v>
+      </c>
+      <c r="P49" s="15">
+        <f t="shared" si="17"/>
+        <v>-4</v>
+      </c>
+      <c r="Q49" s="16">
+        <f t="shared" si="18"/>
+        <v>-18</v>
+      </c>
+      <c r="R49" s="22"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="22"/>
+      <c r="V49" s="22"/>
+      <c r="W49" s="22"/>
+      <c r="X49" s="22"/>
+      <c r="Y49" s="22"/>
+      <c r="Z49" s="22"/>
+      <c r="AA49" s="22"/>
+      <c r="AB49" s="22"/>
+      <c r="AC49" s="22"/>
+      <c r="AD49" s="26"/>
+      <c r="AE49" s="26"/>
+      <c r="AF49" s="26"/>
+      <c r="AG49" s="30"/>
+      <c r="AH49" s="22"/>
+      <c r="AI49" s="22"/>
+      <c r="AJ49" s="22"/>
+      <c r="AK49" s="22"/>
+      <c r="AL49" s="22"/>
+      <c r="AM49" s="22"/>
+      <c r="AN49" s="22"/>
+    </row>
+    <row r="50" spans="1:40" s="11" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="13">
-        <f>SUM(C10:C48)</f>
+      <c r="C50" s="13">
+        <f>SUM(C10:C49)</f>
         <v>109</v>
       </c>
-      <c r="D49" s="13">
-        <f>SUM(D10:D48)</f>
+      <c r="D50" s="13">
+        <f>SUM(D10:D49)</f>
         <v>109</v>
       </c>
-      <c r="E49" s="13">
-        <f>SUM(E10:E48)</f>
+      <c r="E50" s="13">
+        <f>SUM(E10:E49)</f>
         <v>109</v>
       </c>
-      <c r="F49" s="13">
-        <f>SUM(F10:F48)</f>
+      <c r="F50" s="13">
+        <f>SUM(F10:F49)</f>
         <v>109</v>
       </c>
-      <c r="G49" s="19">
-        <f>SUM(G10:G48)/2</f>
-        <v>436</v>
-      </c>
-      <c r="H49" s="13">
-        <f t="shared" ref="H49:Q49" si="15">SUM(H10:H48)</f>
-        <v>12</v>
-      </c>
-      <c r="I49" s="13">
-        <f t="shared" si="15"/>
-        <v>17</v>
-      </c>
-      <c r="J49" s="13">
-        <f t="shared" si="15"/>
-        <v>6</v>
-      </c>
-      <c r="K49" s="13">
-        <f t="shared" si="15"/>
-        <v>11.5</v>
-      </c>
-      <c r="L49" s="20">
-        <f t="shared" si="15"/>
-        <v>46.5</v>
-      </c>
-      <c r="M49" s="13">
-        <f t="shared" si="15"/>
-        <v>-97</v>
-      </c>
-      <c r="N49" s="13">
-        <f t="shared" si="15"/>
-        <v>-92</v>
-      </c>
-      <c r="O49" s="13">
-        <f t="shared" si="15"/>
-        <v>-103</v>
-      </c>
-      <c r="P49" s="13">
-        <f t="shared" si="15"/>
-        <v>-97.5</v>
-      </c>
-      <c r="Q49" s="21">
-        <f t="shared" si="15"/>
-        <v>-389.5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:17" ht="12" thickTop="1" x14ac:dyDescent="0.15"/>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B52" s="37" t="s">
+      <c r="G50" s="19">
+        <f>SUM(G10:G49)/2</f>
+        <v>435</v>
+      </c>
+      <c r="H50" s="13">
+        <f t="shared" ref="H50:Q50" si="19">SUM(H10:H49)</f>
+        <v>19</v>
+      </c>
+      <c r="I50" s="13">
+        <f t="shared" si="19"/>
+        <v>41</v>
+      </c>
+      <c r="J50" s="13">
+        <f t="shared" si="19"/>
+        <v>38</v>
+      </c>
+      <c r="K50" s="13">
+        <f t="shared" si="19"/>
+        <v>18.5</v>
+      </c>
+      <c r="L50" s="20">
+        <f t="shared" si="19"/>
+        <v>116.5</v>
+      </c>
+      <c r="M50" s="13">
+        <f t="shared" si="19"/>
+        <v>-90</v>
+      </c>
+      <c r="N50" s="13">
+        <f t="shared" si="19"/>
+        <v>-68</v>
+      </c>
+      <c r="O50" s="13">
+        <f t="shared" si="19"/>
+        <v>-71</v>
+      </c>
+      <c r="P50" s="13">
+        <f t="shared" si="19"/>
+        <v>-90.5</v>
+      </c>
+      <c r="Q50" s="21">
+        <f t="shared" si="19"/>
+        <v>-319.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B53" s="37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B53" s="36" t="s">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B54" s="36" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B54" s="33" t="s">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B55" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B55" s="35" t="s">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B56" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B56" s="34" t="s">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B57" s="34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B59" s="1" t="s">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B61" s="1" t="s">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B62" s="1" t="s">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B63" s="1" t="s">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B64" s="1" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4161,7 +4285,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
@@ -4174,7 +4298,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>

<commit_message>
Projektplan auf stand gebracht mit Stunden
</commit_message>
<xml_diff>
--- a/Projekt Handbuch/Projektplan.xlsx
+++ b/Projekt Handbuch/Projektplan.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Documents\AlienSoccer\Projekt Handbuch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ursus/Git/AlienHacky/Projekt Handbuch/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
     <author>Stefan Hagen</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP13" authorId="0" shapeId="0">
+    <comment ref="AP13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
   <si>
     <t>Aufwand IST</t>
   </si>
@@ -363,11 +363,17 @@
   <si>
     <t>Grundgerüst</t>
   </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>Sitzungen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0_ ;[Red]\-0.0\ "/>
   </numFmts>
@@ -707,6 +713,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -728,18 +741,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1207,109 +1213,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AP65"/>
+  <dimension ref="A1:AP66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I47" sqref="I47"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" customWidth="1"/>
     <col min="3" max="6" width="4" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="4" style="1" customWidth="1"/>
-    <col min="13" max="17" width="5.42578125" style="1" customWidth="1"/>
-    <col min="18" max="40" width="3.7109375" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="17" width="5.5" style="1" customWidth="1"/>
+    <col min="18" max="40" width="3.6640625" style="1" customWidth="1"/>
+    <col min="41" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:42" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="43" t="s">
+    <row r="8" spans="1:42" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="48" t="s">
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="47">
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="50">
         <v>2016</v>
       </c>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="47"/>
-      <c r="Z8" s="47"/>
-      <c r="AA8" s="47"/>
-      <c r="AB8" s="47"/>
-      <c r="AC8" s="47"/>
-      <c r="AD8" s="47"/>
-      <c r="AE8" s="47"/>
-      <c r="AF8" s="47">
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="50"/>
+      <c r="AA8" s="50"/>
+      <c r="AB8" s="50"/>
+      <c r="AC8" s="50"/>
+      <c r="AD8" s="50"/>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="50">
         <v>2017</v>
       </c>
-      <c r="AG8" s="47"/>
-      <c r="AH8" s="47"/>
-      <c r="AI8" s="47"/>
-      <c r="AJ8" s="47"/>
-      <c r="AK8" s="47"/>
-      <c r="AL8" s="47"/>
-      <c r="AM8" s="47"/>
-      <c r="AN8" s="47"/>
-    </row>
-    <row r="9" spans="1:42" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
-      <c r="B9" s="44"/>
+      <c r="AG8" s="50"/>
+      <c r="AH8" s="50"/>
+      <c r="AI8" s="50"/>
+      <c r="AJ8" s="50"/>
+      <c r="AK8" s="50"/>
+      <c r="AL8" s="50"/>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="50"/>
+    </row>
+    <row r="9" spans="1:42" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="48"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1441,7 +1447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A10" s="24" t="s">
         <v>5</v>
       </c>
@@ -1490,7 +1496,7 @@
       <c r="AM10" s="22"/>
       <c r="AN10" s="22"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
         <v>7</v>
       </c>
@@ -1526,11 +1532,11 @@
         <v>4</v>
       </c>
       <c r="L11" s="9">
-        <f t="shared" ref="L11:L16" si="2">SUM(H11:K11)</f>
+        <f t="shared" ref="L11:L17" si="2">SUM(H11:K11)</f>
         <v>16</v>
       </c>
       <c r="M11" s="15">
-        <f t="shared" ref="M11:P16" si="3">H11-C11</f>
+        <f t="shared" ref="M11:P17" si="3">H11-C11</f>
         <v>0</v>
       </c>
       <c r="N11" s="15">
@@ -1573,7 +1579,7 @@
       <c r="AM11" s="22"/>
       <c r="AN11" s="22"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
         <v>6</v>
       </c>
@@ -1596,21 +1602,25 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="17">
+        <v>2</v>
+      </c>
       <c r="I12" s="17">
         <v>2</v>
       </c>
       <c r="J12" s="17">
         <v>2</v>
       </c>
-      <c r="K12" s="17"/>
+      <c r="K12" s="17">
+        <v>2</v>
+      </c>
       <c r="L12" s="9">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="3"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="N12" s="15">
         <f t="shared" si="3"/>
@@ -1622,11 +1632,11 @@
       </c>
       <c r="P12" s="15">
         <f t="shared" si="3"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="Q12" s="16">
         <f t="shared" si="4"/>
-        <v>-12</v>
+        <v>-8</v>
       </c>
       <c r="R12" s="30"/>
       <c r="S12" s="30"/>
@@ -1652,7 +1662,7 @@
       <c r="AM12" s="22"/>
       <c r="AN12" s="22"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
         <v>8</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1819,7 @@
       <c r="AM14" s="22"/>
       <c r="AN14" s="22"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
@@ -1892,7 +1902,7 @@
       <c r="AM15" s="22"/>
       <c r="AN15" s="22"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>70</v>
       </c>
@@ -1909,17 +1919,19 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="17">
+        <v>4</v>
+      </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M16" s="15">
         <f t="shared" si="3"/>
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="3"/>
@@ -1935,7 +1947,7 @@
       </c>
       <c r="Q16" s="16">
         <f t="shared" si="4"/>
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="38"/>
@@ -1961,20 +1973,48 @@
       <c r="AM16" s="22"/>
       <c r="AN16" s="22"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="15"/>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="17">
+        <v>15</v>
+      </c>
+      <c r="D17" s="17">
+        <v>15</v>
+      </c>
+      <c r="E17" s="17">
+        <v>15</v>
+      </c>
+      <c r="F17" s="17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="10">
+        <v>60</v>
+      </c>
+      <c r="H17" s="17">
+        <v>6</v>
+      </c>
+      <c r="I17" s="17">
+        <v>6</v>
+      </c>
+      <c r="J17" s="17">
+        <v>6</v>
+      </c>
+      <c r="K17" s="17">
+        <v>6</v>
+      </c>
+      <c r="L17" s="9">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="M17" s="15">
+        <f t="shared" si="3"/>
+        <v>-9</v>
+      </c>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
@@ -2003,21 +2043,14 @@
       <c r="AM17" s="22"/>
       <c r="AN17" s="22"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>31</v>
-      </c>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A18" s="18"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="32">
-        <f>SUM(G19:G26)</f>
-        <v>76</v>
-      </c>
+      <c r="G18" s="10"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
@@ -2052,56 +2085,34 @@
       <c r="AM18" s="22"/>
       <c r="AN18" s="22"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>73</v>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A19" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="28">
-        <v>10</v>
-      </c>
-      <c r="G19" s="10">
-        <f t="shared" ref="G19:G26" si="5">SUM(C19:F19)</f>
-        <v>10</v>
+      <c r="F19" s="17"/>
+      <c r="G19" s="32">
+        <f>SUM(G20:G27)</f>
+        <v>76</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="17">
-        <v>1</v>
-      </c>
-      <c r="L19" s="9">
-        <f t="shared" ref="L19:L26" si="6">SUM(H19:K19)</f>
-        <v>1</v>
-      </c>
-      <c r="M19" s="15">
-        <f t="shared" ref="M19:P26" si="7">H19-C19</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="15">
-        <f t="shared" si="7"/>
-        <v>-9</v>
-      </c>
-      <c r="Q19" s="16">
-        <f t="shared" ref="Q19:Q26" si="8">SUM(M19:P19)</f>
-        <v>-9</v>
-      </c>
-      <c r="R19" s="31"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
       <c r="U19" s="23"/>
       <c r="V19" s="23"/>
       <c r="W19" s="23"/>
@@ -2123,37 +2134,35 @@
       <c r="AM19" s="22"/>
       <c r="AN19" s="22"/>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="17">
+        <v>73</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="28">
         <v>10</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
       <c r="G20" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="G20:G27" si="5">SUM(C20:F20)</f>
         <v>10</v>
       </c>
       <c r="H20" s="17"/>
-      <c r="I20" s="17">
-        <v>10</v>
-      </c>
-      <c r="J20" s="17">
-        <v>1</v>
-      </c>
-      <c r="K20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17">
+        <v>3</v>
+      </c>
       <c r="L20" s="9">
-        <f t="shared" si="6"/>
-        <v>11</v>
+        <f t="shared" ref="L20:L27" si="6">SUM(H20:K20)</f>
+        <v>3</v>
       </c>
       <c r="M20" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="M20:P27" si="7">H20-C20</f>
         <v>0</v>
       </c>
       <c r="N20" s="15">
@@ -2162,19 +2171,19 @@
       </c>
       <c r="O20" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="Q20" s="16">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="R20" s="40"/>
-      <c r="S20" s="40"/>
-      <c r="T20" s="40"/>
+        <f t="shared" ref="Q20:Q27" si="8">SUM(M20:P20)</f>
+        <v>-7</v>
+      </c>
+      <c r="R20" s="31"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
       <c r="U20" s="23"/>
       <c r="V20" s="23"/>
       <c r="W20" s="23"/>
@@ -2196,12 +2205,12 @@
       <c r="AM20" s="22"/>
       <c r="AN20" s="22"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="17">
@@ -2215,13 +2224,15 @@
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17">
-        <v>5</v>
-      </c>
-      <c r="J21" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="J21" s="17">
+        <v>1</v>
+      </c>
       <c r="K21" s="17"/>
       <c r="L21" s="9">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M21" s="15">
         <f t="shared" si="7"/>
@@ -2229,11 +2240,11 @@
       </c>
       <c r="N21" s="15">
         <f t="shared" si="7"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="O21" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="15">
         <f t="shared" si="7"/>
@@ -2241,13 +2252,13 @@
       </c>
       <c r="Q21" s="16">
         <f t="shared" si="8"/>
-        <v>-5</v>
-      </c>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="40"/>
-      <c r="V21" s="40"/>
+        <v>1</v>
+      </c>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
       <c r="W21" s="23"/>
       <c r="X21" s="23"/>
       <c r="Y21" s="23"/>
@@ -2267,30 +2278,32 @@
       <c r="AM21" s="22"/>
       <c r="AN21" s="22"/>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A22" s="42" t="s">
-        <v>15</v>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A22" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+        <v>34</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="17">
+        <v>10</v>
+      </c>
       <c r="E22" s="17"/>
-      <c r="F22" s="28">
-        <v>5</v>
-      </c>
+      <c r="F22" s="17"/>
       <c r="G22" s="10">
         <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17">
         <v>5</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M22" s="15">
         <f t="shared" si="7"/>
@@ -2298,7 +2311,7 @@
       </c>
       <c r="N22" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="O22" s="15">
         <f t="shared" si="7"/>
@@ -2306,7 +2319,7 @@
       </c>
       <c r="P22" s="15">
         <f t="shared" si="7"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="16">
         <f t="shared" si="8"/>
@@ -2315,8 +2328,8 @@
       <c r="R22" s="23"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
-      <c r="U22" s="39"/>
-      <c r="V22" s="39"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="40"/>
       <c r="W22" s="23"/>
       <c r="X22" s="23"/>
       <c r="Y22" s="23"/>
@@ -2336,65 +2349,61 @@
       <c r="AM22" s="22"/>
       <c r="AN22" s="22"/>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
-        <v>16</v>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A23" s="42" t="s">
+        <v>15</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="17">
-        <v>2</v>
-      </c>
-      <c r="D23" s="17">
-        <v>10</v>
-      </c>
-      <c r="E23" s="17">
-        <v>10</v>
-      </c>
-      <c r="F23" s="17"/>
+        <v>35</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="28">
+        <v>5</v>
+      </c>
       <c r="G23" s="10">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="H23" s="17"/>
-      <c r="I23" s="17">
-        <v>6</v>
-      </c>
+      <c r="I23" s="17"/>
       <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="K23" s="17">
+        <v>3</v>
+      </c>
       <c r="L23" s="9">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M23" s="15">
         <f t="shared" si="7"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="7"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="O23" s="15">
         <f t="shared" si="7"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="P23" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Q23" s="16">
         <f t="shared" si="8"/>
-        <v>-16</v>
+        <v>-2</v>
       </c>
       <c r="R23" s="23"/>
       <c r="S23" s="23"/>
       <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="40"/>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="38"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
       <c r="Z23" s="23"/>
       <c r="AA23" s="23"/>
       <c r="AB23" s="23"/>
@@ -2411,45 +2420,48 @@
       <c r="AM23" s="22"/>
       <c r="AN23" s="22"/>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="C24" s="17">
+        <v>2</v>
+      </c>
+      <c r="D24" s="17">
+        <v>10</v>
+      </c>
       <c r="E24" s="17">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="10">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17">
-        <f>7+2+1+1.5+3.5</f>
-        <v>15</v>
-      </c>
+      <c r="I24" s="17">
+        <v>6</v>
+      </c>
+      <c r="J24" s="17"/>
       <c r="K24" s="17"/>
       <c r="L24" s="9">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="M24" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="N24" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="O24" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="P24" s="15">
         <f t="shared" si="7"/>
@@ -2457,16 +2469,16 @@
       </c>
       <c r="Q24" s="16">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
+        <v>-16</v>
+      </c>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
       <c r="T24" s="23"/>
       <c r="U24" s="23"/>
       <c r="V24" s="23"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="23"/>
-      <c r="Y24" s="23"/>
+      <c r="W24" s="40"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="38"/>
       <c r="Z24" s="23"/>
       <c r="AA24" s="23"/>
       <c r="AB24" s="23"/>
@@ -2483,30 +2495,33 @@
       <c r="AM24" s="22"/>
       <c r="AN24" s="22"/>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17">
-        <v>2</v>
-      </c>
+      <c r="E25" s="17">
+        <v>14</v>
+      </c>
+      <c r="F25" s="17"/>
       <c r="G25" s="10">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
+      <c r="J25" s="17">
+        <f>7+2+1+1.5+3.5</f>
+        <v>15</v>
+      </c>
       <c r="K25" s="17"/>
       <c r="L25" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M25" s="15">
         <f t="shared" si="7"/>
@@ -2518,24 +2533,24 @@
       </c>
       <c r="O25" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" s="15">
         <f t="shared" si="7"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="16">
         <f t="shared" si="8"/>
-        <v>-2</v>
-      </c>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="39"/>
-      <c r="U25" s="39"/>
+        <v>1</v>
+      </c>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
       <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
+      <c r="W25" s="41"/>
       <c r="X25" s="23"/>
-      <c r="Y25" s="39"/>
+      <c r="Y25" s="23"/>
       <c r="Z25" s="23"/>
       <c r="AA25" s="23"/>
       <c r="AB25" s="23"/>
@@ -2552,30 +2567,32 @@
       <c r="AM25" s="22"/>
       <c r="AN25" s="22"/>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" s="10">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
+      <c r="K26" s="17">
+        <v>1</v>
+      </c>
       <c r="L26" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="15">
         <f t="shared" si="7"/>
@@ -2591,22 +2608,22 @@
       </c>
       <c r="P26" s="15">
         <f t="shared" si="7"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="Q26" s="16">
         <f t="shared" si="8"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="R26" s="23"/>
       <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
+      <c r="T26" s="39"/>
+      <c r="U26" s="39"/>
       <c r="V26" s="23"/>
       <c r="W26" s="23"/>
       <c r="X26" s="23"/>
-      <c r="Y26" s="23"/>
-      <c r="Z26" s="39"/>
-      <c r="AA26" s="39"/>
+      <c r="Y26" s="39"/>
+      <c r="Z26" s="23"/>
+      <c r="AA26" s="23"/>
       <c r="AB26" s="23"/>
       <c r="AC26" s="23"/>
       <c r="AD26" s="26"/>
@@ -2621,24 +2638,51 @@
       <c r="AM26" s="22"/>
       <c r="AN26" s="22"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="25"/>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A27" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="10"/>
+      <c r="F27" s="17">
+        <v>3</v>
+      </c>
+      <c r="G27" s="10">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="16"/>
+      <c r="L27" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="15">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="Q27" s="16">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
       <c r="R27" s="23"/>
       <c r="S27" s="23"/>
       <c r="T27" s="23"/>
@@ -2647,8 +2691,8 @@
       <c r="W27" s="23"/>
       <c r="X27" s="23"/>
       <c r="Y27" s="23"/>
-      <c r="Z27" s="23"/>
-      <c r="AA27" s="23"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="39"/>
       <c r="AB27" s="23"/>
       <c r="AC27" s="23"/>
       <c r="AD27" s="26"/>
@@ -2663,21 +2707,14 @@
       <c r="AM27" s="22"/>
       <c r="AN27" s="22"/>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A28" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>36</v>
-      </c>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A28" s="18"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="32">
-        <f>SUM(G29:G32)</f>
-        <v>104</v>
-      </c>
+      <c r="G28" s="10"/>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
@@ -2712,61 +2749,39 @@
       <c r="AM28" s="22"/>
       <c r="AN28" s="22"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="17">
-        <v>10</v>
-      </c>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A29" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
-      <c r="F29" s="17">
-        <v>30</v>
-      </c>
-      <c r="G29" s="10">
-        <f>SUM(C29:F29)</f>
-        <v>40</v>
+      <c r="F29" s="17"/>
+      <c r="G29" s="32">
+        <f>SUM(G30:G33)</f>
+        <v>104</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
-      <c r="L29" s="9">
-        <f>SUM(H29:K29)</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="15">
-        <f t="shared" ref="M29:P32" si="9">H29-C29</f>
-        <v>-10</v>
-      </c>
-      <c r="N29" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="15">
-        <f t="shared" si="9"/>
-        <v>-30</v>
-      </c>
-      <c r="Q29" s="16">
-        <f>SUM(M29:P29)</f>
-        <v>-40</v>
-      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="16"/>
       <c r="R29" s="23"/>
       <c r="S29" s="23"/>
       <c r="T29" s="23"/>
       <c r="U29" s="23"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="38"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
       <c r="Z29" s="23"/>
       <c r="AA29" s="23"/>
       <c r="AB29" s="23"/>
@@ -2783,22 +2798,24 @@
       <c r="AM29" s="22"/>
       <c r="AN29" s="22"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="29">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="C30" s="17">
+        <v>10</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
+      <c r="F30" s="17">
+        <v>30</v>
+      </c>
       <c r="G30" s="10">
         <f>SUM(C30:F30)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
@@ -2809,8 +2826,8 @@
         <v>0</v>
       </c>
       <c r="M30" s="15">
-        <f t="shared" si="9"/>
-        <v>-20</v>
+        <f t="shared" ref="M30:P33" si="9">H30-C30</f>
+        <v>-10</v>
       </c>
       <c r="N30" s="15">
         <f t="shared" si="9"/>
@@ -2822,20 +2839,20 @@
       </c>
       <c r="P30" s="15">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="Q30" s="16">
         <f>SUM(M30:P30)</f>
-        <v>-20</v>
+        <v>-40</v>
       </c>
       <c r="R30" s="23"/>
       <c r="S30" s="23"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="23"/>
-      <c r="Y30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="39"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="38"/>
       <c r="Z30" s="23"/>
       <c r="AA30" s="23"/>
       <c r="AB30" s="23"/>
@@ -2852,34 +2869,38 @@
       <c r="AM30" s="22"/>
       <c r="AN30" s="22"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="29">
         <v>20</v>
       </c>
-      <c r="B31" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="29"/>
       <c r="D31" s="17"/>
-      <c r="E31" s="17">
-        <v>18</v>
-      </c>
+      <c r="E31" s="17"/>
       <c r="F31" s="17"/>
       <c r="G31" s="10">
         <f>SUM(C31:F31)</f>
-        <v>18</v>
-      </c>
-      <c r="H31" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="H31" s="17">
+        <v>12</v>
+      </c>
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
+      <c r="K31" s="17">
+        <v>2</v>
+      </c>
       <c r="L31" s="9">
         <f>SUM(H31:K31)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M31" s="15">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="N31" s="15">
         <f t="shared" si="9"/>
@@ -2887,23 +2908,23 @@
       </c>
       <c r="O31" s="15">
         <f t="shared" si="9"/>
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="P31" s="15">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q31" s="16">
         <f>SUM(M31:P31)</f>
-        <v>-18</v>
+        <v>-6</v>
       </c>
       <c r="R31" s="23"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="41"/>
-      <c r="W31" s="41"/>
-      <c r="X31" s="41"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="38"/>
+      <c r="U31" s="38"/>
+      <c r="V31" s="23"/>
+      <c r="W31" s="23"/>
+      <c r="X31" s="23"/>
       <c r="Y31" s="23"/>
       <c r="Z31" s="23"/>
       <c r="AA31" s="23"/>
@@ -2921,24 +2942,22 @@
       <c r="AM31" s="22"/>
       <c r="AN31" s="22"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17">
-        <v>20</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="17">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="10">
         <f>SUM(C32:F32)</f>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
@@ -2954,11 +2973,11 @@
       </c>
       <c r="N32" s="15">
         <f t="shared" si="9"/>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="O32" s="15">
         <f t="shared" si="9"/>
-        <v>-6</v>
+        <v>-18</v>
       </c>
       <c r="P32" s="15">
         <f t="shared" si="9"/>
@@ -2966,20 +2985,20 @@
       </c>
       <c r="Q32" s="16">
         <f>SUM(M32:P32)</f>
-        <v>-26</v>
-      </c>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
-      <c r="U32" s="22"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="40"/>
-      <c r="Z32" s="40"/>
-      <c r="AA32" s="40"/>
-      <c r="AB32" s="41"/>
-      <c r="AC32" s="22"/>
+        <v>-18</v>
+      </c>
+      <c r="R32" s="23"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
       <c r="AD32" s="26"/>
       <c r="AE32" s="26"/>
       <c r="AF32" s="26"/>
@@ -2992,65 +3011,65 @@
       <c r="AM32" s="22"/>
       <c r="AN32" s="22"/>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A33" s="50" t="s">
-        <v>93</v>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A33" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
+      <c r="D33" s="17">
+        <v>20</v>
+      </c>
       <c r="E33" s="17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="10">
-        <f>C33+D33+E33+F33</f>
-        <v>2</v>
+        <f>SUM(C33:F33)</f>
+        <v>26</v>
       </c>
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
-      <c r="J33" s="17">
-        <v>2</v>
-      </c>
+      <c r="J33" s="17"/>
       <c r="K33" s="17"/>
       <c r="L33" s="9">
         <f>SUM(H33:K33)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M33" s="15">
-        <f t="shared" ref="M33" si="10">H33-C33</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N33" s="15">
-        <f t="shared" ref="N33" si="11">I33-D33</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>-20</v>
       </c>
       <c r="O33" s="15">
-        <f t="shared" ref="O33" si="12">J33-E33</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>-6</v>
       </c>
       <c r="P33" s="15">
-        <f t="shared" ref="P33" si="13">K33-F33</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q33" s="16">
         <f>SUM(M33:P33)</f>
-        <v>0</v>
+        <v>-26</v>
       </c>
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
-      <c r="U33" s="52"/>
+      <c r="U33" s="22"/>
       <c r="V33" s="23"/>
-      <c r="W33" s="31"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="51"/>
-      <c r="Z33" s="51"/>
-      <c r="AA33" s="51"/>
-      <c r="AB33" s="51"/>
-      <c r="AC33" s="31"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="40"/>
+      <c r="Z33" s="40"/>
+      <c r="AA33" s="40"/>
+      <c r="AB33" s="41"/>
+      <c r="AC33" s="22"/>
       <c r="AD33" s="26"/>
       <c r="AE33" s="26"/>
       <c r="AF33" s="26"/>
@@ -3063,36 +3082,65 @@
       <c r="AM33" s="22"/>
       <c r="AN33" s="22"/>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="25"/>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A34" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>94</v>
+      </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
+      <c r="E34" s="17">
+        <v>2</v>
+      </c>
       <c r="F34" s="17"/>
-      <c r="G34" s="10"/>
+      <c r="G34" s="10">
+        <f>C34+D34+E34+F34</f>
+        <v>2</v>
+      </c>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="J34" s="17">
+        <v>2</v>
+      </c>
       <c r="K34" s="17"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="16"/>
+      <c r="L34" s="9">
+        <f>SUM(H34:K34)</f>
+        <v>2</v>
+      </c>
+      <c r="M34" s="15">
+        <f t="shared" ref="M34" si="10">H34-C34</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="15">
+        <f t="shared" ref="N34" si="11">I34-D34</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="15">
+        <f t="shared" ref="O34" si="12">J34-E34</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="15">
+        <f t="shared" ref="P34" si="13">K34-F34</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="16">
+        <f>SUM(M34:P34)</f>
+        <v>0</v>
+      </c>
       <c r="R34" s="22"/>
       <c r="S34" s="22"/>
       <c r="T34" s="22"/>
-      <c r="U34" s="22"/>
-      <c r="V34" s="22"/>
-      <c r="W34" s="22"/>
-      <c r="X34" s="22"/>
-      <c r="Y34" s="22"/>
-      <c r="Z34" s="22"/>
-      <c r="AA34" s="22"/>
-      <c r="AB34" s="22"/>
-      <c r="AC34" s="22"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="23"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="44"/>
+      <c r="Z34" s="44"/>
+      <c r="AA34" s="44"/>
+      <c r="AB34" s="44"/>
+      <c r="AC34" s="31"/>
       <c r="AD34" s="26"/>
       <c r="AE34" s="26"/>
       <c r="AF34" s="26"/>
@@ -3105,21 +3153,14 @@
       <c r="AM34" s="22"/>
       <c r="AN34" s="22"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>41</v>
-      </c>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A35" s="18"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
-      <c r="G35" s="32">
-        <f>SUM(G36:G37)</f>
-        <v>32</v>
-      </c>
+      <c r="G35" s="10"/>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
@@ -3154,70 +3195,36 @@
       <c r="AM35" s="22"/>
       <c r="AN35" s="22"/>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="17">
-        <v>4</v>
-      </c>
-      <c r="D36" s="17">
-        <v>4</v>
-      </c>
-      <c r="E36" s="17">
-        <v>4</v>
-      </c>
-      <c r="F36" s="17">
-        <v>4</v>
-      </c>
-      <c r="G36" s="10">
-        <f>SUM(C36:F36)</f>
-        <v>16</v>
-      </c>
-      <c r="H36" s="17">
-        <v>2</v>
-      </c>
-      <c r="I36" s="17">
-        <v>2</v>
-      </c>
-      <c r="J36" s="17">
-        <v>2</v>
-      </c>
-      <c r="K36" s="17">
-        <v>2</v>
-      </c>
-      <c r="L36" s="9">
-        <f>SUM(H36:K36)</f>
-        <v>8</v>
-      </c>
-      <c r="M36" s="15">
-        <f t="shared" ref="M36:P37" si="14">H36-C36</f>
-        <v>-2</v>
-      </c>
-      <c r="N36" s="15">
-        <f t="shared" si="14"/>
-        <v>-2</v>
-      </c>
-      <c r="O36" s="15">
-        <f t="shared" si="14"/>
-        <v>-2</v>
-      </c>
-      <c r="P36" s="15">
-        <f t="shared" si="14"/>
-        <v>-2</v>
-      </c>
-      <c r="Q36" s="16">
-        <f>SUM(M36:P36)</f>
-        <v>-8</v>
-      </c>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A36" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="32">
+        <f>SUM(G37:G38)</f>
+        <v>32</v>
+      </c>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="16"/>
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="22"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
       <c r="W36" s="22"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="22"/>
@@ -3237,12 +3244,12 @@
       <c r="AM36" s="22"/>
       <c r="AN36" s="22"/>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A37" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="17">
         <v>4</v>
@@ -3277,7 +3284,7 @@
         <v>8</v>
       </c>
       <c r="M37" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="M37:P38" si="14">H37-C37</f>
         <v>-2</v>
       </c>
       <c r="N37" s="15">
@@ -3320,29 +3327,70 @@
       <c r="AM37" s="22"/>
       <c r="AN37" s="22"/>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="16"/>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A38" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="17">
+        <v>4</v>
+      </c>
+      <c r="D38" s="17">
+        <v>4</v>
+      </c>
+      <c r="E38" s="17">
+        <v>4</v>
+      </c>
+      <c r="F38" s="17">
+        <v>4</v>
+      </c>
+      <c r="G38" s="10">
+        <f>SUM(C38:F38)</f>
+        <v>16</v>
+      </c>
+      <c r="H38" s="17">
+        <v>2</v>
+      </c>
+      <c r="I38" s="17">
+        <v>2</v>
+      </c>
+      <c r="J38" s="17">
+        <v>2</v>
+      </c>
+      <c r="K38" s="17">
+        <v>2</v>
+      </c>
+      <c r="L38" s="9">
+        <f>SUM(H38:K38)</f>
+        <v>8</v>
+      </c>
+      <c r="M38" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="N38" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="O38" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="P38" s="15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+      <c r="Q38" s="16">
+        <f>SUM(M38:P38)</f>
+        <v>-8</v>
+      </c>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
-      <c r="U38" s="23"/>
-      <c r="V38" s="23"/>
+      <c r="U38" s="30"/>
+      <c r="V38" s="30"/>
       <c r="W38" s="22"/>
       <c r="X38" s="22"/>
       <c r="Y38" s="22"/>
@@ -3362,29 +3410,19 @@
       <c r="AM38" s="22"/>
       <c r="AN38" s="22"/>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A39" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>71</v>
-      </c>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A39" s="18"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
-      <c r="G39" s="32">
-        <f>SUM(G40:G41)</f>
-        <v>48</v>
-      </c>
+      <c r="G39" s="10"/>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
-      <c r="L39" s="9">
-        <f>SUM(H39:K39)</f>
-        <v>0</v>
-      </c>
+      <c r="L39" s="9"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
@@ -3393,8 +3431,8 @@
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="22"/>
-      <c r="U39" s="22"/>
-      <c r="V39" s="22"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="23"/>
       <c r="W39" s="22"/>
       <c r="X39" s="22"/>
       <c r="Y39" s="22"/>
@@ -3414,28 +3452,20 @@
       <c r="AM39" s="22"/>
       <c r="AN39" s="22"/>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="17">
-        <v>10</v>
-      </c>
-      <c r="D40" s="17">
-        <v>10</v>
-      </c>
-      <c r="E40" s="17">
-        <v>10</v>
-      </c>
-      <c r="F40" s="17">
-        <v>10</v>
-      </c>
-      <c r="G40" s="10">
-        <f>SUM(C40:F40)</f>
-        <v>40</v>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A40" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="32">
+        <f>SUM(G41:G42)</f>
+        <v>48</v>
       </c>
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
@@ -3445,38 +3475,23 @@
         <f>SUM(H40:K40)</f>
         <v>0</v>
       </c>
-      <c r="M40" s="15">
-        <f t="shared" ref="M40:P41" si="15">H40-C40</f>
-        <v>-10</v>
-      </c>
-      <c r="N40" s="15">
-        <f t="shared" si="15"/>
-        <v>-10</v>
-      </c>
-      <c r="O40" s="15">
-        <f t="shared" si="15"/>
-        <v>-10</v>
-      </c>
-      <c r="P40" s="15">
-        <f t="shared" si="15"/>
-        <v>-10</v>
-      </c>
-      <c r="Q40" s="16">
-        <f>SUM(M40:P40)</f>
-        <v>-40</v>
-      </c>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="16"/>
       <c r="R40" s="22"/>
       <c r="S40" s="22"/>
-      <c r="T40" s="23"/>
-      <c r="U40" s="23"/>
-      <c r="V40" s="30"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="22"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="22"/>
+      <c r="X40" s="22"/>
+      <c r="Y40" s="22"/>
+      <c r="Z40" s="22"/>
+      <c r="AA40" s="22"/>
+      <c r="AB40" s="22"/>
+      <c r="AC40" s="22"/>
       <c r="AD40" s="26"/>
       <c r="AE40" s="26"/>
       <c r="AF40" s="26"/>
@@ -3489,28 +3504,28 @@
       <c r="AM40" s="22"/>
       <c r="AN40" s="22"/>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A41" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C41" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D41" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E41" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F41" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G41" s="10">
         <f>SUM(C41:F41)</f>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
@@ -3521,24 +3536,24 @@
         <v>0</v>
       </c>
       <c r="M41" s="15">
-        <f t="shared" si="15"/>
-        <v>-2</v>
+        <f t="shared" ref="M41:P42" si="15">H41-C41</f>
+        <v>-10</v>
       </c>
       <c r="N41" s="15">
         <f t="shared" si="15"/>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="O41" s="15">
         <f t="shared" si="15"/>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="P41" s="15">
         <f t="shared" si="15"/>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="Q41" s="16">
         <f>SUM(M41:P41)</f>
-        <v>-8</v>
+        <v>-40</v>
       </c>
       <c r="R41" s="22"/>
       <c r="S41" s="22"/>
@@ -3564,24 +3579,57 @@
       <c r="AM41" s="22"/>
       <c r="AN41" s="22"/>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="10"/>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A42" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="17">
+        <v>2</v>
+      </c>
+      <c r="D42" s="17">
+        <v>2</v>
+      </c>
+      <c r="E42" s="17">
+        <v>2</v>
+      </c>
+      <c r="F42" s="17">
+        <v>2</v>
+      </c>
+      <c r="G42" s="10">
+        <f>SUM(C42:F42)</f>
+        <v>8</v>
+      </c>
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="16"/>
+      <c r="L42" s="9">
+        <f>SUM(H42:K42)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="N42" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="O42" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="P42" s="15">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+      <c r="Q42" s="16">
+        <f>SUM(M42:P42)</f>
+        <v>-8</v>
+      </c>
       <c r="R42" s="22"/>
       <c r="S42" s="22"/>
       <c r="T42" s="23"/>
@@ -3606,21 +3654,14 @@
       <c r="AM42" s="22"/>
       <c r="AN42" s="22"/>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>44</v>
-      </c>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A43" s="18"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
-      <c r="G43" s="32">
-        <f>SUM(G44:G49)</f>
-        <v>106</v>
-      </c>
+      <c r="G43" s="10"/>
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
@@ -3633,16 +3674,16 @@
       <c r="Q43" s="16"/>
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
-      <c r="T43" s="22"/>
-      <c r="U43" s="22"/>
-      <c r="V43" s="22"/>
-      <c r="W43" s="22"/>
-      <c r="X43" s="22"/>
-      <c r="Y43" s="22"/>
-      <c r="Z43" s="22"/>
-      <c r="AA43" s="22"/>
-      <c r="AB43" s="22"/>
-      <c r="AC43" s="22"/>
+      <c r="T43" s="23"/>
+      <c r="U43" s="23"/>
+      <c r="V43" s="30"/>
+      <c r="W43" s="30"/>
+      <c r="X43" s="30"/>
+      <c r="Y43" s="30"/>
+      <c r="Z43" s="30"/>
+      <c r="AA43" s="30"/>
+      <c r="AB43" s="30"/>
+      <c r="AC43" s="30"/>
       <c r="AD43" s="26"/>
       <c r="AE43" s="26"/>
       <c r="AF43" s="26"/>
@@ -3655,68 +3696,34 @@
       <c r="AM43" s="22"/>
       <c r="AN43" s="22"/>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="17">
-        <v>3</v>
-      </c>
-      <c r="D44" s="17">
-        <v>2</v>
-      </c>
-      <c r="E44" s="17">
-        <v>2</v>
-      </c>
-      <c r="F44" s="17">
-        <v>2</v>
-      </c>
-      <c r="G44" s="10">
-        <f t="shared" ref="G44:G49" si="16">SUM(C44:F44)</f>
-        <v>9</v>
-      </c>
-      <c r="H44" s="17">
-        <v>2</v>
-      </c>
-      <c r="I44" s="17">
-        <v>1</v>
-      </c>
-      <c r="J44" s="17">
-        <v>1</v>
-      </c>
-      <c r="K44" s="17">
-        <v>1</v>
-      </c>
-      <c r="L44" s="9">
-        <f>SUM(H44:K44)</f>
-        <v>5</v>
-      </c>
-      <c r="M44" s="15">
-        <f t="shared" ref="M44:P49" si="17">H44-C44</f>
-        <v>-1</v>
-      </c>
-      <c r="N44" s="15">
-        <f t="shared" si="17"/>
-        <v>-1</v>
-      </c>
-      <c r="O44" s="15">
-        <f t="shared" si="17"/>
-        <v>-1</v>
-      </c>
-      <c r="P44" s="15">
-        <f t="shared" si="17"/>
-        <v>-1</v>
-      </c>
-      <c r="Q44" s="16">
-        <f t="shared" ref="Q44:Q49" si="18">SUM(M44:P44)</f>
-        <v>-4</v>
-      </c>
-      <c r="R44" s="30"/>
-      <c r="S44" s="30"/>
-      <c r="T44" s="30"/>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A44" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="32">
+        <f>SUM(G45:G50)</f>
+        <v>106</v>
+      </c>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="22"/>
       <c r="U44" s="22"/>
       <c r="V44" s="22"/>
       <c r="W44" s="22"/>
@@ -3738,69 +3745,77 @@
       <c r="AM44" s="22"/>
       <c r="AN44" s="22"/>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A45" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C45" s="17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D45" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E45" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F45" s="17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G45" s="10">
-        <f t="shared" si="16"/>
-        <v>24</v>
-      </c>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17"/>
+        <f t="shared" ref="G45:G50" si="16">SUM(C45:F45)</f>
+        <v>9</v>
+      </c>
+      <c r="H45" s="17">
+        <v>2</v>
+      </c>
+      <c r="I45" s="17">
+        <v>1</v>
+      </c>
+      <c r="J45" s="17">
+        <v>1</v>
+      </c>
+      <c r="K45" s="17">
+        <v>1</v>
+      </c>
       <c r="L45" s="9">
-        <f>SUM(H45:K45)</f>
-        <v>0</v>
+        <f t="shared" ref="L45:L50" si="17">SUM(H45:K45)</f>
+        <v>5</v>
       </c>
       <c r="M45" s="15">
-        <f t="shared" si="17"/>
-        <v>-6</v>
+        <f t="shared" ref="M45:P50" si="18">H45-C45</f>
+        <v>-1</v>
       </c>
       <c r="N45" s="15">
-        <f t="shared" si="17"/>
-        <v>-6</v>
+        <f t="shared" si="18"/>
+        <v>-1</v>
       </c>
       <c r="O45" s="15">
-        <f t="shared" si="17"/>
-        <v>-6</v>
+        <f t="shared" si="18"/>
+        <v>-1</v>
       </c>
       <c r="P45" s="15">
-        <f t="shared" si="17"/>
-        <v>-6</v>
+        <f t="shared" si="18"/>
+        <v>-1</v>
       </c>
       <c r="Q45" s="16">
-        <f t="shared" si="18"/>
-        <v>-24</v>
-      </c>
-      <c r="R45" s="22"/>
-      <c r="S45" s="22"/>
-      <c r="T45" s="22"/>
+        <f t="shared" ref="Q45:Q50" si="19">SUM(M45:P45)</f>
+        <v>-4</v>
+      </c>
+      <c r="R45" s="30"/>
+      <c r="S45" s="30"/>
+      <c r="T45" s="30"/>
       <c r="U45" s="22"/>
       <c r="V45" s="22"/>
       <c r="W45" s="22"/>
       <c r="X45" s="22"/>
       <c r="Y45" s="22"/>
-      <c r="Z45" s="30"/>
-      <c r="AA45" s="30"/>
-      <c r="AB45" s="30"/>
-      <c r="AC45" s="30"/>
+      <c r="Z45" s="22"/>
+      <c r="AA45" s="22"/>
+      <c r="AB45" s="22"/>
+      <c r="AC45" s="22"/>
       <c r="AD45" s="26"/>
       <c r="AE45" s="26"/>
       <c r="AF45" s="26"/>
@@ -3813,73 +3828,65 @@
       <c r="AM45" s="22"/>
       <c r="AN45" s="22"/>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A46" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C46" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D46" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E46" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F46" s="17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G46" s="10">
         <f t="shared" si="16"/>
-        <v>40</v>
-      </c>
-      <c r="H46" s="17">
-        <v>2</v>
-      </c>
-      <c r="I46" s="17">
-        <v>4</v>
-      </c>
-      <c r="J46" s="17">
-        <v>4</v>
-      </c>
-      <c r="K46" s="17">
-        <v>2.5</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
       <c r="L46" s="9">
-        <f>SUM(H46:K46)</f>
-        <v>12.5</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="M46" s="15">
-        <f t="shared" si="17"/>
-        <v>-8</v>
+        <f t="shared" si="18"/>
+        <v>-6</v>
       </c>
       <c r="N46" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-6</v>
       </c>
       <c r="O46" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-6</v>
       </c>
       <c r="P46" s="15">
-        <f t="shared" si="17"/>
-        <v>-7.5</v>
+        <f t="shared" si="18"/>
+        <v>-6</v>
       </c>
       <c r="Q46" s="16">
-        <f t="shared" si="18"/>
-        <v>-27.5</v>
-      </c>
-      <c r="R46" s="30"/>
-      <c r="S46" s="30"/>
-      <c r="T46" s="30"/>
-      <c r="U46" s="30"/>
-      <c r="V46" s="30"/>
-      <c r="W46" s="30"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="30"/>
+        <f t="shared" si="19"/>
+        <v>-24</v>
+      </c>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
+      <c r="U46" s="22"/>
+      <c r="V46" s="22"/>
+      <c r="W46" s="22"/>
+      <c r="X46" s="22"/>
+      <c r="Y46" s="22"/>
       <c r="Z46" s="30"/>
       <c r="AA46" s="30"/>
       <c r="AB46" s="30"/>
@@ -3896,77 +3903,77 @@
       <c r="AM46" s="22"/>
       <c r="AN46" s="22"/>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A47" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C47" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D47" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E47" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G47" s="10">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="H47" s="17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I47" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J47" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K47" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L47" s="9">
-        <f>SUM(H47:K47)</f>
-        <v>5</v>
+        <f t="shared" si="17"/>
+        <v>16</v>
       </c>
       <c r="M47" s="15">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>-6</v>
       </c>
       <c r="N47" s="15">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>-6</v>
       </c>
       <c r="O47" s="15">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>-6</v>
       </c>
       <c r="P47" s="15">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>-6</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="R47" s="22"/>
+        <f t="shared" si="19"/>
+        <v>-24</v>
+      </c>
+      <c r="R47" s="30"/>
       <c r="S47" s="30"/>
-      <c r="T47" s="22"/>
-      <c r="U47" s="22"/>
-      <c r="V47" s="22"/>
-      <c r="W47" s="22"/>
-      <c r="X47" s="22"/>
-      <c r="Y47" s="22"/>
-      <c r="Z47" s="22"/>
-      <c r="AA47" s="22"/>
-      <c r="AB47" s="22"/>
-      <c r="AC47" s="22"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="30"/>
+      <c r="V47" s="30"/>
+      <c r="W47" s="30"/>
+      <c r="X47" s="30"/>
+      <c r="Y47" s="30"/>
+      <c r="Z47" s="30"/>
+      <c r="AA47" s="30"/>
+      <c r="AB47" s="30"/>
+      <c r="AC47" s="30"/>
       <c r="AD47" s="26"/>
       <c r="AE47" s="26"/>
       <c r="AF47" s="26"/>
@@ -3979,70 +3986,70 @@
       <c r="AM47" s="22"/>
       <c r="AN47" s="22"/>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A48" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D48" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48" s="10">
         <f t="shared" si="16"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H48" s="17">
         <v>3</v>
       </c>
       <c r="I48" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J48" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K48" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L48" s="9">
-        <f>SUM(H48:K48)</f>
-        <v>12</v>
+        <f t="shared" si="17"/>
+        <v>6</v>
       </c>
       <c r="M48" s="15">
-        <f t="shared" si="17"/>
-        <v>-1</v>
+        <f t="shared" si="18"/>
+        <v>1</v>
       </c>
       <c r="N48" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="O48" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="16">
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="O48" s="15">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="P48" s="15">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="Q48" s="16">
-        <f t="shared" si="18"/>
-        <v>2</v>
-      </c>
       <c r="R48" s="22"/>
-      <c r="S48" s="22"/>
+      <c r="S48" s="30"/>
       <c r="T48" s="22"/>
       <c r="U48" s="22"/>
-      <c r="V48" s="30"/>
+      <c r="V48" s="22"/>
       <c r="W48" s="22"/>
       <c r="X48" s="22"/>
       <c r="Y48" s="22"/>
@@ -4062,62 +4069,70 @@
       <c r="AM48" s="22"/>
       <c r="AN48" s="22"/>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A49" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D49" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E49" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F49" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G49" s="10">
         <f t="shared" si="16"/>
-        <v>18</v>
-      </c>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17"/>
-      <c r="K49" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="H49" s="17">
+        <v>3</v>
+      </c>
+      <c r="I49" s="17">
+        <v>3</v>
+      </c>
+      <c r="J49" s="17">
+        <v>3</v>
+      </c>
+      <c r="K49" s="17">
+        <v>3</v>
+      </c>
       <c r="L49" s="9">
-        <f>SUM(H49:K49)</f>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>12</v>
       </c>
       <c r="M49" s="15">
-        <f t="shared" si="17"/>
-        <v>-6</v>
+        <f t="shared" si="18"/>
+        <v>-1</v>
       </c>
       <c r="N49" s="15">
-        <f t="shared" si="17"/>
-        <v>-4</v>
+        <f t="shared" si="18"/>
+        <v>1</v>
       </c>
       <c r="O49" s="15">
-        <f t="shared" si="17"/>
-        <v>-4</v>
+        <f t="shared" si="18"/>
+        <v>1</v>
       </c>
       <c r="P49" s="15">
-        <f t="shared" si="17"/>
-        <v>-4</v>
+        <f t="shared" si="18"/>
+        <v>1</v>
       </c>
       <c r="Q49" s="16">
-        <f t="shared" si="18"/>
-        <v>-18</v>
+        <f t="shared" si="19"/>
+        <v>2</v>
       </c>
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
       <c r="T49" s="22"/>
       <c r="U49" s="22"/>
-      <c r="V49" s="22"/>
+      <c r="V49" s="30"/>
       <c r="W49" s="22"/>
       <c r="X49" s="22"/>
       <c r="Y49" s="22"/>
@@ -4128,7 +4143,7 @@
       <c r="AD49" s="26"/>
       <c r="AE49" s="26"/>
       <c r="AF49" s="26"/>
-      <c r="AG49" s="30"/>
+      <c r="AG49" s="22"/>
       <c r="AH49" s="22"/>
       <c r="AI49" s="22"/>
       <c r="AJ49" s="22"/>
@@ -4137,124 +4152,199 @@
       <c r="AM49" s="22"/>
       <c r="AN49" s="22"/>
     </row>
-    <row r="50" spans="1:40" s="11" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="12" t="s">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A50" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="17">
+        <v>6</v>
+      </c>
+      <c r="D50" s="17">
+        <v>4</v>
+      </c>
+      <c r="E50" s="17">
+        <v>4</v>
+      </c>
+      <c r="F50" s="17">
+        <v>4</v>
+      </c>
+      <c r="G50" s="10">
+        <f t="shared" si="16"/>
+        <v>18</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="9">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M50" s="15">
+        <f t="shared" si="18"/>
+        <v>-6</v>
+      </c>
+      <c r="N50" s="15">
+        <f t="shared" si="18"/>
+        <v>-4</v>
+      </c>
+      <c r="O50" s="15">
+        <f t="shared" si="18"/>
+        <v>-4</v>
+      </c>
+      <c r="P50" s="15">
+        <f t="shared" si="18"/>
+        <v>-4</v>
+      </c>
+      <c r="Q50" s="16">
+        <f t="shared" si="19"/>
+        <v>-18</v>
+      </c>
+      <c r="R50" s="22"/>
+      <c r="S50" s="22"/>
+      <c r="T50" s="22"/>
+      <c r="U50" s="22"/>
+      <c r="V50" s="22"/>
+      <c r="W50" s="22"/>
+      <c r="X50" s="22"/>
+      <c r="Y50" s="22"/>
+      <c r="Z50" s="22"/>
+      <c r="AA50" s="22"/>
+      <c r="AB50" s="22"/>
+      <c r="AC50" s="22"/>
+      <c r="AD50" s="26"/>
+      <c r="AE50" s="26"/>
+      <c r="AF50" s="26"/>
+      <c r="AG50" s="30"/>
+      <c r="AH50" s="22"/>
+      <c r="AI50" s="22"/>
+      <c r="AJ50" s="22"/>
+      <c r="AK50" s="22"/>
+      <c r="AL50" s="22"/>
+      <c r="AM50" s="22"/>
+      <c r="AN50" s="22"/>
+    </row>
+    <row r="51" spans="1:40" s="11" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="13">
-        <f>SUM(C10:C49)</f>
-        <v>109</v>
-      </c>
-      <c r="D50" s="13">
-        <f>SUM(D10:D49)</f>
-        <v>109</v>
-      </c>
-      <c r="E50" s="13">
-        <f>SUM(E10:E49)</f>
-        <v>109</v>
-      </c>
-      <c r="F50" s="13">
-        <f>SUM(F10:F49)</f>
-        <v>109</v>
-      </c>
-      <c r="G50" s="19">
-        <f>SUM(G10:G49)/2</f>
-        <v>435</v>
-      </c>
-      <c r="H50" s="13">
-        <f t="shared" ref="H50:Q50" si="19">SUM(H10:H49)</f>
-        <v>19</v>
-      </c>
-      <c r="I50" s="13">
-        <f t="shared" si="19"/>
-        <v>41</v>
-      </c>
-      <c r="J50" s="13">
-        <f t="shared" si="19"/>
-        <v>38</v>
-      </c>
-      <c r="K50" s="13">
-        <f t="shared" si="19"/>
-        <v>18.5</v>
-      </c>
-      <c r="L50" s="20">
-        <f t="shared" si="19"/>
-        <v>116.5</v>
-      </c>
-      <c r="M50" s="13">
-        <f t="shared" si="19"/>
-        <v>-90</v>
-      </c>
-      <c r="N50" s="13">
-        <f t="shared" si="19"/>
+      <c r="C51" s="13">
+        <f>SUM(C10:C50)</f>
+        <v>124</v>
+      </c>
+      <c r="D51" s="13">
+        <f>SUM(D10:D50)</f>
+        <v>124</v>
+      </c>
+      <c r="E51" s="13">
+        <f>SUM(E10:E50)</f>
+        <v>124</v>
+      </c>
+      <c r="F51" s="13">
+        <f>SUM(F10:F50)</f>
+        <v>124</v>
+      </c>
+      <c r="G51" s="19">
+        <f>SUM(G10:G50)/2</f>
+        <v>465</v>
+      </c>
+      <c r="H51" s="13">
+        <f t="shared" ref="H51:Q51" si="20">SUM(H10:H50)</f>
+        <v>46</v>
+      </c>
+      <c r="I51" s="13">
+        <f t="shared" si="20"/>
+        <v>47</v>
+      </c>
+      <c r="J51" s="13">
+        <f t="shared" si="20"/>
+        <v>44</v>
+      </c>
+      <c r="K51" s="13">
+        <f t="shared" si="20"/>
+        <v>36</v>
+      </c>
+      <c r="L51" s="20">
+        <f t="shared" si="20"/>
+        <v>173</v>
+      </c>
+      <c r="M51" s="13">
+        <f t="shared" si="20"/>
+        <v>-78</v>
+      </c>
+      <c r="N51" s="13">
+        <f t="shared" si="20"/>
         <v>-68</v>
       </c>
-      <c r="O50" s="13">
-        <f t="shared" si="19"/>
+      <c r="O51" s="13">
+        <f t="shared" si="20"/>
         <v>-71</v>
       </c>
-      <c r="P50" s="13">
-        <f t="shared" si="19"/>
-        <v>-90.5</v>
-      </c>
-      <c r="Q50" s="21">
-        <f t="shared" si="19"/>
-        <v>-319.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:40" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B53" s="37" t="s">
+      <c r="P51" s="13">
+        <f t="shared" si="20"/>
+        <v>-79</v>
+      </c>
+      <c r="Q51" s="21">
+        <f t="shared" si="20"/>
+        <v>-287</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" ht="12" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="54" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B54" s="37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B54" s="36" t="s">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B55" s="36" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B55" s="33" t="s">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B56" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B56" s="35" t="s">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B57" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B57" s="34" t="s">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B58" s="34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B61" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B61" s="1" t="s">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B62" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B62" s="1" t="s">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B63" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B63" s="1" t="s">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="B64" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B65" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B66" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4285,7 +4375,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
@@ -4298,7 +4388,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>